<commit_message>
adicionando log e perguntas filtro
</commit_message>
<xml_diff>
--- a/database/troubleshooting.xlsx
+++ b/database/troubleshooting.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq - Copy\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B6BD104-1D7E-4716-92C7-94480F77AC34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3714512-827F-4250-8959-612905BCC5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="994" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="997" uniqueCount="118">
   <si>
     <t>interface</t>
   </si>
@@ -370,6 +370,15 @@
   </si>
   <si>
     <t>smq915</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coletor não funciona,não liga,não pega,parou de funcionar </t>
+  </si>
+  <si>
+    <t>coletor travando,parado,travado,não funciona,não pega</t>
   </si>
 </sst>
 </file>
@@ -797,10 +806,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E221B1-E974-48EE-8D2F-4D47A5EBE7F7}">
-  <dimension ref="A1:J168"/>
+  <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A169" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -809,15 +818,15 @@
     <col min="2" max="2" width="29.140625" customWidth="1"/>
     <col min="3" max="3" width="26.85546875" customWidth="1"/>
     <col min="4" max="4" width="23.28515625" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
-    <col min="6" max="6" width="25.42578125" customWidth="1"/>
-    <col min="8" max="8" width="11" customWidth="1"/>
-    <col min="9" max="10" width="38.85546875" customWidth="1"/>
-    <col min="12" max="12" width="8.140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="38.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="34.5703125" customWidth="1"/>
+    <col min="7" max="7" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="11" customWidth="1"/>
+    <col min="10" max="11" width="38.85546875" customWidth="1"/>
+    <col min="13" max="13" width="8.140625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>7</v>
       </c>
@@ -834,10 +843,13 @@
         <v>2</v>
       </c>
       <c r="F1" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="39.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="54" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>8</v>
       </c>
@@ -854,10 +866,13 @@
         <v>12</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+        <v>116</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="54" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>8</v>
       </c>
@@ -874,10 +889,13 @@
         <v>13</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -893,11 +911,12 @@
       <c r="E4" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
@@ -913,11 +932,12 @@
       <c r="E5" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="F5" s="3"/>
+      <c r="G5" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
         <v>8</v>
       </c>
@@ -933,11 +953,12 @@
       <c r="E6" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+      <c r="F6" s="3"/>
+      <c r="G6" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>8</v>
       </c>
@@ -953,11 +974,12 @@
       <c r="E7" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+      <c r="F7" s="3"/>
+      <c r="G7" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>8</v>
       </c>
@@ -973,11 +995,12 @@
       <c r="E8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="F8" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" ht="36" x14ac:dyDescent="0.35">
+      <c r="F8" s="3"/>
+      <c r="G8" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -993,12 +1016,13 @@
       <c r="E9" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="F9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J9" s="1"/>
-    </row>
-    <row r="10" spans="1:10" ht="36" x14ac:dyDescent="0.35">
+      <c r="F9" s="3"/>
+      <c r="G9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K9" s="1"/>
+    </row>
+    <row r="10" spans="1:11" ht="36" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>8</v>
       </c>
@@ -1014,12 +1038,13 @@
       <c r="E10" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J10" s="1"/>
-    </row>
-    <row r="11" spans="1:10" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F10" s="3"/>
+      <c r="G10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K10" s="1"/>
+    </row>
+    <row r="11" spans="1:11" ht="33.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3" t="s">
         <v>8</v>
       </c>
@@ -1035,12 +1060,13 @@
       <c r="E11" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J11" s="1"/>
-    </row>
-    <row r="12" spans="1:10" ht="36" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F11" s="3"/>
+      <c r="G11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" spans="1:11" ht="36" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
         <v>8</v>
       </c>
@@ -1056,12 +1082,13 @@
       <c r="E12" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J12" s="1"/>
-    </row>
-    <row r="13" spans="1:10" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F12" s="3"/>
+      <c r="G12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K12" s="1"/>
+    </row>
+    <row r="13" spans="1:11" ht="29.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>8</v>
       </c>
@@ -1077,12 +1104,13 @@
       <c r="E13" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="J13" s="1"/>
-    </row>
-    <row r="14" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="F13" s="3"/>
+      <c r="G13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="K13" s="1"/>
+    </row>
+    <row r="14" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
         <v>8</v>
       </c>
@@ -1098,11 +1126,12 @@
       <c r="E14" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F14" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" ht="18" x14ac:dyDescent="0.25">
+      <c r="F14" s="3"/>
+      <c r="G14" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>8</v>
       </c>
@@ -1118,11 +1147,12 @@
       <c r="E15" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F15" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" ht="36" x14ac:dyDescent="0.25">
+      <c r="F15" s="3"/>
+      <c r="G15" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>8</v>
       </c>
@@ -1138,11 +1168,12 @@
       <c r="E16" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F16" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F16" s="3"/>
+      <c r="G16" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
         <v>8</v>
       </c>
@@ -1158,11 +1189,12 @@
       <c r="E17" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F17" s="3"/>
+      <c r="G17" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>8</v>
       </c>
@@ -1178,11 +1210,12 @@
       <c r="E18" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F18" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F18" s="3"/>
+      <c r="G18" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>8</v>
       </c>
@@ -1198,11 +1231,12 @@
       <c r="E19" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F19" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F19" s="3"/>
+      <c r="G19" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>8</v>
       </c>
@@ -1218,11 +1252,12 @@
       <c r="E20" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="F20" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F20" s="3"/>
+      <c r="G20" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>8</v>
       </c>
@@ -1238,11 +1273,12 @@
       <c r="E21" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F21" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F21" s="3"/>
+      <c r="G21" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>8</v>
       </c>
@@ -1258,11 +1294,12 @@
       <c r="E22" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="F22" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F22" s="3"/>
+      <c r="G22" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>8</v>
       </c>
@@ -1278,11 +1315,12 @@
       <c r="E23" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="F23" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F23" s="3"/>
+      <c r="G23" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>8</v>
       </c>
@@ -1298,11 +1336,12 @@
       <c r="E24" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="F24" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F24" s="3"/>
+      <c r="G24" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>8</v>
       </c>
@@ -1318,11 +1357,12 @@
       <c r="E25" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="F25" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F25" s="3"/>
+      <c r="G25" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>8</v>
       </c>
@@ -1338,11 +1378,12 @@
       <c r="E26" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F26" s="3"/>
+      <c r="G26" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>8</v>
       </c>
@@ -1358,11 +1399,12 @@
       <c r="E27" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="F27" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F27" s="3"/>
+      <c r="G27" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
         <v>8</v>
       </c>
@@ -1378,11 +1420,12 @@
       <c r="E28" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="F28" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F28" s="3"/>
+      <c r="G28" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>8</v>
       </c>
@@ -1398,11 +1441,12 @@
       <c r="E29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="F29" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F29" s="3"/>
+      <c r="G29" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
         <v>8</v>
       </c>
@@ -1418,11 +1462,12 @@
       <c r="E30" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F30" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F30" s="3"/>
+      <c r="G30" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>37</v>
       </c>
@@ -1438,11 +1483,12 @@
       <c r="E31" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F31" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F31" s="3"/>
+      <c r="G31" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
@@ -1458,11 +1504,12 @@
       <c r="E32" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F32" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F32" s="3"/>
+      <c r="G32" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>37</v>
       </c>
@@ -1478,11 +1525,12 @@
       <c r="E33" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F33" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F33" s="3"/>
+      <c r="G33" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>37</v>
       </c>
@@ -1498,11 +1546,12 @@
       <c r="E34" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F34" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F34" s="3"/>
+      <c r="G34" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>37</v>
       </c>
@@ -1518,11 +1567,12 @@
       <c r="E35" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F35" s="3"/>
+      <c r="G35" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>37</v>
       </c>
@@ -1538,11 +1588,12 @@
       <c r="E36" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="F36" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F36" s="3"/>
+      <c r="G36" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>37</v>
       </c>
@@ -1558,11 +1609,12 @@
       <c r="E37" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F37" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F37" s="3"/>
+      <c r="G37" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>37</v>
       </c>
@@ -1578,11 +1630,12 @@
       <c r="E38" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F38" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F38" s="3"/>
+      <c r="G38" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>37</v>
       </c>
@@ -1598,11 +1651,12 @@
       <c r="E39" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F39" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F39" s="3"/>
+      <c r="G39" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>37</v>
       </c>
@@ -1618,11 +1672,12 @@
       <c r="E40" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F40" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F40" s="3"/>
+      <c r="G40" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>37</v>
       </c>
@@ -1638,11 +1693,12 @@
       <c r="E41" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F41" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F41" s="3"/>
+      <c r="G41" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>37</v>
       </c>
@@ -1658,11 +1714,12 @@
       <c r="E42" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F42" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F42" s="3"/>
+      <c r="G42" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>37</v>
       </c>
@@ -1678,11 +1735,12 @@
       <c r="E43" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F43" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F43" s="3"/>
+      <c r="G43" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>37</v>
       </c>
@@ -1698,11 +1756,12 @@
       <c r="E44" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F44" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F44" s="3"/>
+      <c r="G44" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>37</v>
       </c>
@@ -1718,11 +1777,12 @@
       <c r="E45" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F45" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F45" s="3"/>
+      <c r="G45" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
         <v>37</v>
       </c>
@@ -1738,11 +1798,12 @@
       <c r="E46" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="F46" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F46" s="3"/>
+      <c r="G46" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>56</v>
       </c>
@@ -1758,11 +1819,12 @@
       <c r="E47" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F47" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F47" s="3"/>
+      <c r="G47" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>56</v>
       </c>
@@ -1778,11 +1840,12 @@
       <c r="E48" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F48" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="49" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F48" s="3"/>
+      <c r="G48" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
         <v>56</v>
       </c>
@@ -1798,11 +1861,12 @@
       <c r="E49" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F49" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F49" s="3"/>
+      <c r="G49" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>56</v>
       </c>
@@ -1818,11 +1882,12 @@
       <c r="E50" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F50" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="51" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F50" s="3"/>
+      <c r="G50" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>56</v>
       </c>
@@ -1838,11 +1903,12 @@
       <c r="E51" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F51" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="52" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F51" s="3"/>
+      <c r="G51" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>56</v>
       </c>
@@ -1858,11 +1924,12 @@
       <c r="E52" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F52" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F52" s="3"/>
+      <c r="G52" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>56</v>
       </c>
@@ -1878,11 +1945,12 @@
       <c r="E53" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F53" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F53" s="3"/>
+      <c r="G53" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>56</v>
       </c>
@@ -1898,11 +1966,12 @@
       <c r="E54" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F54" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F54" s="3"/>
+      <c r="G54" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
         <v>56</v>
       </c>
@@ -1918,11 +1987,12 @@
       <c r="E55" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F55" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="56" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F55" s="3"/>
+      <c r="G55" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>56</v>
       </c>
@@ -1938,11 +2008,12 @@
       <c r="E56" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F56" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F56" s="3"/>
+      <c r="G56" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>56</v>
       </c>
@@ -1958,11 +2029,12 @@
       <c r="E57" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F57" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F57" s="3"/>
+      <c r="G57" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
         <v>56</v>
       </c>
@@ -1978,11 +2050,12 @@
       <c r="E58" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F58" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="59" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F58" s="3"/>
+      <c r="G58" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>56</v>
       </c>
@@ -1998,11 +2071,12 @@
       <c r="E59" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F59" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F59" s="3"/>
+      <c r="G59" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>56</v>
       </c>
@@ -2018,11 +2092,12 @@
       <c r="E60" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F60" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F60" s="3"/>
+      <c r="G60" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>56</v>
       </c>
@@ -2038,11 +2113,12 @@
       <c r="E61" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F61" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="62" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F61" s="3"/>
+      <c r="G61" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="62" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>56</v>
       </c>
@@ -2058,11 +2134,12 @@
       <c r="E62" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F62" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F62" s="3"/>
+      <c r="G62" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="63" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>56</v>
       </c>
@@ -2078,11 +2155,12 @@
       <c r="E63" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F63" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F63" s="3"/>
+      <c r="G63" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>56</v>
       </c>
@@ -2098,11 +2176,12 @@
       <c r="E64" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F64" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F64" s="3"/>
+      <c r="G64" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="65" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>56</v>
       </c>
@@ -2118,11 +2197,12 @@
       <c r="E65" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F65" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F65" s="3"/>
+      <c r="G65" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="66" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>56</v>
       </c>
@@ -2138,11 +2218,12 @@
       <c r="E66" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F66" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="67" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F66" s="3"/>
+      <c r="G66" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="67" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>56</v>
       </c>
@@ -2158,11 +2239,12 @@
       <c r="E67" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F67" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F67" s="3"/>
+      <c r="G67" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="68" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>56</v>
       </c>
@@ -2178,11 +2260,12 @@
       <c r="E68" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F68" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F68" s="3"/>
+      <c r="G68" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="69" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>56</v>
       </c>
@@ -2198,11 +2281,12 @@
       <c r="E69" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F69" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F69" s="3"/>
+      <c r="G69" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="70" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>56</v>
       </c>
@@ -2218,11 +2302,12 @@
       <c r="E70" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F70" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F70" s="3"/>
+      <c r="G70" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="71" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>56</v>
       </c>
@@ -2238,11 +2323,12 @@
       <c r="E71" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F71" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F71" s="3"/>
+      <c r="G71" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="72" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>56</v>
       </c>
@@ -2258,11 +2344,12 @@
       <c r="E72" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F72" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F72" s="3"/>
+      <c r="G72" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="73" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>56</v>
       </c>
@@ -2278,11 +2365,12 @@
       <c r="E73" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F73" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F73" s="3"/>
+      <c r="G73" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="74" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>56</v>
       </c>
@@ -2298,11 +2386,12 @@
       <c r="E74" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F74" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F74" s="3"/>
+      <c r="G74" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="75" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
         <v>56</v>
       </c>
@@ -2318,11 +2407,12 @@
       <c r="E75" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F75" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F75" s="3"/>
+      <c r="G75" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="76" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
         <v>56</v>
       </c>
@@ -2338,11 +2428,12 @@
       <c r="E76" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F76" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F76" s="3"/>
+      <c r="G76" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="77" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
         <v>56</v>
       </c>
@@ -2358,11 +2449,12 @@
       <c r="E77" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F77" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F77" s="3"/>
+      <c r="G77" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="78" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
         <v>56</v>
       </c>
@@ -2378,11 +2470,12 @@
       <c r="E78" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F78" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F78" s="3"/>
+      <c r="G78" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="79" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
         <v>56</v>
       </c>
@@ -2398,11 +2491,12 @@
       <c r="E79" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F79" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F79" s="3"/>
+      <c r="G79" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="80" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
         <v>56</v>
       </c>
@@ -2418,11 +2512,12 @@
       <c r="E80" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F80" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F80" s="3"/>
+      <c r="G80" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="81" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>56</v>
       </c>
@@ -2438,11 +2533,12 @@
       <c r="E81" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F81" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F81" s="3"/>
+      <c r="G81" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="82" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="3" t="s">
         <v>56</v>
       </c>
@@ -2458,11 +2554,12 @@
       <c r="E82" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F82" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F82" s="3"/>
+      <c r="G82" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="83" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>56</v>
       </c>
@@ -2478,11 +2575,12 @@
       <c r="E83" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F83" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F83" s="3"/>
+      <c r="G83" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="84" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>56</v>
       </c>
@@ -2498,11 +2596,12 @@
       <c r="E84" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F84" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="85" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F84" s="3"/>
+      <c r="G84" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="85" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>56</v>
       </c>
@@ -2518,11 +2617,12 @@
       <c r="E85" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F85" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F85" s="3"/>
+      <c r="G85" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="86" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>56</v>
       </c>
@@ -2538,11 +2638,12 @@
       <c r="E86" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F86" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F86" s="3"/>
+      <c r="G86" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="87" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>56</v>
       </c>
@@ -2558,11 +2659,12 @@
       <c r="E87" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F87" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F87" s="3"/>
+      <c r="G87" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="88" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A88" s="3" t="s">
         <v>96</v>
       </c>
@@ -2578,11 +2680,12 @@
       <c r="E88" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="F88" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F88" s="3"/>
+      <c r="G88" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="89" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A89" s="3" t="s">
         <v>96</v>
       </c>
@@ -2598,11 +2701,12 @@
       <c r="E89" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F89" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F89" s="3"/>
+      <c r="G89" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="90" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
         <v>96</v>
       </c>
@@ -2618,11 +2722,12 @@
       <c r="E90" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F90" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F90" s="3"/>
+      <c r="G90" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="91" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A91" s="3" t="s">
         <v>96</v>
       </c>
@@ -2638,11 +2743,12 @@
       <c r="E91" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="F91" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F91" s="3"/>
+      <c r="G91" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="92" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A92" s="3" t="s">
         <v>96</v>
       </c>
@@ -2658,11 +2764,12 @@
       <c r="E92" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F92" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F92" s="3"/>
+      <c r="G92" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="93" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A93" s="3" t="s">
         <v>96</v>
       </c>
@@ -2678,11 +2785,12 @@
       <c r="E93" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F93" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F93" s="3"/>
+      <c r="G93" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="94" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A94" s="3" t="s">
         <v>96</v>
       </c>
@@ -2698,11 +2806,12 @@
       <c r="E94" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F94" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F94" s="3"/>
+      <c r="G94" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="95" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>96</v>
       </c>
@@ -2718,11 +2827,12 @@
       <c r="E95" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F95" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F95" s="3"/>
+      <c r="G95" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="96" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A96" s="3" t="s">
         <v>96</v>
       </c>
@@ -2738,11 +2848,12 @@
       <c r="E96" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F96" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F96" s="3"/>
+      <c r="G96" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="97" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A97" s="3" t="s">
         <v>96</v>
       </c>
@@ -2758,11 +2869,12 @@
       <c r="E97" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F97" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F97" s="3"/>
+      <c r="G97" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="98" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
         <v>96</v>
       </c>
@@ -2778,11 +2890,12 @@
       <c r="E98" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F98" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F98" s="3"/>
+      <c r="G98" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="99" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
         <v>96</v>
       </c>
@@ -2798,11 +2911,12 @@
       <c r="E99" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F99" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F99" s="3"/>
+      <c r="G99" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="100" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="3" t="s">
         <v>96</v>
       </c>
@@ -2818,11 +2932,12 @@
       <c r="E100" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F100" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F100" s="3"/>
+      <c r="G100" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="101" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A101" s="3" t="s">
         <v>96</v>
       </c>
@@ -2838,11 +2953,12 @@
       <c r="E101" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F101" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F101" s="3"/>
+      <c r="G101" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="102" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A102" s="3" t="s">
         <v>96</v>
       </c>
@@ -2858,11 +2974,12 @@
       <c r="E102" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F102" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F102" s="3"/>
+      <c r="G102" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="103" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A103" s="3" t="s">
         <v>96</v>
       </c>
@@ -2878,11 +2995,12 @@
       <c r="E103" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F103" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F103" s="3"/>
+      <c r="G103" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="104" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A104" s="3" t="s">
         <v>96</v>
       </c>
@@ -2898,11 +3016,12 @@
       <c r="E104" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F104" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F104" s="3"/>
+      <c r="G104" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="105" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A105" s="3" t="s">
         <v>96</v>
       </c>
@@ -2918,11 +3037,12 @@
       <c r="E105" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F105" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F105" s="3"/>
+      <c r="G105" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="106" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A106" s="3" t="s">
         <v>96</v>
       </c>
@@ -2938,11 +3058,12 @@
       <c r="E106" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F106" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F106" s="3"/>
+      <c r="G106" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="107" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A107" s="3" t="s">
         <v>96</v>
       </c>
@@ -2958,11 +3079,12 @@
       <c r="E107" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F107" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F107" s="3"/>
+      <c r="G107" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="108" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A108" s="3" t="s">
         <v>96</v>
       </c>
@@ -2978,11 +3100,12 @@
       <c r="E108" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F108" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F108" s="3"/>
+      <c r="G108" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="109" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="3" t="s">
         <v>96</v>
       </c>
@@ -2998,11 +3121,12 @@
       <c r="E109" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F109" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="110" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F109" s="3"/>
+      <c r="G109" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="110" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A110" s="3" t="s">
         <v>96</v>
       </c>
@@ -3018,11 +3142,12 @@
       <c r="E110" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F110" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F110" s="3"/>
+      <c r="G110" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="111" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A111" s="3" t="s">
         <v>96</v>
       </c>
@@ -3038,11 +3163,12 @@
       <c r="E111" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="F111" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F111" s="3"/>
+      <c r="G111" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="112" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A112" s="3" t="s">
         <v>96</v>
       </c>
@@ -3058,11 +3184,12 @@
       <c r="E112" s="3" t="s">
         <v>79</v>
       </c>
-      <c r="F112" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F112" s="3"/>
+      <c r="G112" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="113" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="3" t="s">
         <v>96</v>
       </c>
@@ -3078,11 +3205,12 @@
       <c r="E113" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F113" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F113" s="3"/>
+      <c r="G113" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="114" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="3" t="s">
         <v>96</v>
       </c>
@@ -3098,11 +3226,12 @@
       <c r="E114" s="3" t="s">
         <v>81</v>
       </c>
-      <c r="F114" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F114" s="3"/>
+      <c r="G114" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="115" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A115" s="3" t="s">
         <v>96</v>
       </c>
@@ -3118,11 +3247,12 @@
       <c r="E115" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="F115" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F115" s="3"/>
+      <c r="G115" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="116" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A116" s="3" t="s">
         <v>96</v>
       </c>
@@ -3138,11 +3268,12 @@
       <c r="E116" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F116" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="117" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F116" s="3"/>
+      <c r="G116" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="117" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A117" s="3" t="s">
         <v>96</v>
       </c>
@@ -3158,11 +3289,12 @@
       <c r="E117" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="F117" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="118" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F117" s="3"/>
+      <c r="G117" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="118" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A118" s="3" t="s">
         <v>96</v>
       </c>
@@ -3178,11 +3310,12 @@
       <c r="E118" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="F118" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="119" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F118" s="3"/>
+      <c r="G118" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="119" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A119" s="3" t="s">
         <v>96</v>
       </c>
@@ -3198,11 +3331,12 @@
       <c r="E119" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F119" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="120" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F119" s="3"/>
+      <c r="G119" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="120" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="3" t="s">
         <v>96</v>
       </c>
@@ -3218,11 +3352,12 @@
       <c r="E120" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F120" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F120" s="3"/>
+      <c r="G120" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="121" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A121" s="3" t="s">
         <v>96</v>
       </c>
@@ -3238,11 +3373,12 @@
       <c r="E121" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F121" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="122" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F121" s="3"/>
+      <c r="G121" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="122" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A122" s="3" t="s">
         <v>96</v>
       </c>
@@ -3258,11 +3394,12 @@
       <c r="E122" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F122" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="123" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F122" s="3"/>
+      <c r="G122" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="123" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="3" t="s">
         <v>96</v>
       </c>
@@ -3278,11 +3415,12 @@
       <c r="E123" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F123" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F123" s="3"/>
+      <c r="G123" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A124" s="3" t="s">
         <v>96</v>
       </c>
@@ -3298,11 +3436,12 @@
       <c r="E124" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F124" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="125" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F124" s="3"/>
+      <c r="G124" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="125" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A125" s="3" t="s">
         <v>96</v>
       </c>
@@ -3318,11 +3457,12 @@
       <c r="E125" s="3" t="s">
         <v>91</v>
       </c>
-      <c r="F125" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="126" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F125" s="3"/>
+      <c r="G125" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="126" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="3" t="s">
         <v>96</v>
       </c>
@@ -3338,11 +3478,12 @@
       <c r="E126" s="3" t="s">
         <v>92</v>
       </c>
-      <c r="F126" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="127" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F126" s="3"/>
+      <c r="G126" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="127" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A127" s="3" t="s">
         <v>96</v>
       </c>
@@ -3358,11 +3499,12 @@
       <c r="E127" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="F127" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="128" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F127" s="3"/>
+      <c r="G127" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="128" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A128" s="3" t="s">
         <v>96</v>
       </c>
@@ -3378,11 +3520,12 @@
       <c r="E128" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="F128" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="129" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F128" s="3"/>
+      <c r="G128" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="129" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A129" s="3" t="s">
         <v>9</v>
       </c>
@@ -3398,11 +3541,12 @@
       <c r="E129" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F129" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="130" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F129" s="3"/>
+      <c r="G129" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="130" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A130" s="3" t="s">
         <v>9</v>
       </c>
@@ -3418,11 +3562,12 @@
       <c r="E130" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F130" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="131" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F130" s="3"/>
+      <c r="G130" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="131" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A131" s="3" t="s">
         <v>9</v>
       </c>
@@ -3438,11 +3583,12 @@
       <c r="E131" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F131" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="132" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F131" s="3"/>
+      <c r="G131" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="132" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A132" s="3" t="s">
         <v>9</v>
       </c>
@@ -3458,11 +3604,12 @@
       <c r="E132" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F132" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="133" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F132" s="3"/>
+      <c r="G132" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="133" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A133" s="3" t="s">
         <v>9</v>
       </c>
@@ -3478,11 +3625,12 @@
       <c r="E133" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F133" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="134" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F133" s="3"/>
+      <c r="G133" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="134" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A134" s="3" t="s">
         <v>9</v>
       </c>
@@ -3498,11 +3646,12 @@
       <c r="E134" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F134" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="135" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F134" s="3"/>
+      <c r="G134" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="135" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A135" s="3" t="s">
         <v>9</v>
       </c>
@@ -3518,11 +3667,12 @@
       <c r="E135" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F135" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="136" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F135" s="3"/>
+      <c r="G135" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="136" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A136" s="3" t="s">
         <v>9</v>
       </c>
@@ -3538,11 +3688,12 @@
       <c r="E136" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F136" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="137" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F136" s="3"/>
+      <c r="G136" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="137" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A137" s="3" t="s">
         <v>9</v>
       </c>
@@ -3558,11 +3709,12 @@
       <c r="E137" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F137" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="138" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F137" s="3"/>
+      <c r="G137" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="138" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A138" s="3" t="s">
         <v>9</v>
       </c>
@@ -3578,11 +3730,12 @@
       <c r="E138" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F138" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="139" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F138" s="3"/>
+      <c r="G138" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="139" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A139" s="3" t="s">
         <v>9</v>
       </c>
@@ -3598,11 +3751,12 @@
       <c r="E139" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F139" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="140" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F139" s="3"/>
+      <c r="G139" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="140" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A140" s="3" t="s">
         <v>9</v>
       </c>
@@ -3618,11 +3772,12 @@
       <c r="E140" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F140" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="141" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F140" s="3"/>
+      <c r="G140" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="141" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A141" s="3" t="s">
         <v>9</v>
       </c>
@@ -3638,11 +3793,12 @@
       <c r="E141" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F141" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="142" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F141" s="3"/>
+      <c r="G141" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="142" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A142" s="3" t="s">
         <v>9</v>
       </c>
@@ -3658,11 +3814,12 @@
       <c r="E142" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F142" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="143" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F142" s="3"/>
+      <c r="G142" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="143" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A143" s="3" t="s">
         <v>9</v>
       </c>
@@ -3678,11 +3835,12 @@
       <c r="E143" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F143" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="144" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F143" s="3"/>
+      <c r="G143" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="144" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A144" s="3" t="s">
         <v>9</v>
       </c>
@@ -3698,11 +3856,12 @@
       <c r="E144" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F144" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="145" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F144" s="3"/>
+      <c r="G144" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="145" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>9</v>
       </c>
@@ -3718,11 +3877,12 @@
       <c r="E145" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F145" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="146" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F145" s="3"/>
+      <c r="G145" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="146" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>9</v>
       </c>
@@ -3738,11 +3898,12 @@
       <c r="E146" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F146" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="147" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F146" s="3"/>
+      <c r="G146" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="147" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>9</v>
       </c>
@@ -3758,11 +3919,12 @@
       <c r="E147" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="F147" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="148" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F147" s="3"/>
+      <c r="G147" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="148" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="3" t="s">
         <v>9</v>
       </c>
@@ -3778,11 +3940,12 @@
       <c r="E148" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="F148" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="149" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F148" s="3"/>
+      <c r="G148" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="149" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="3" t="s">
         <v>9</v>
       </c>
@@ -3798,11 +3961,12 @@
       <c r="E149" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="F149" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="150" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F149" s="3"/>
+      <c r="G149" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="150" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A150" s="3" t="s">
         <v>9</v>
       </c>
@@ -3818,11 +3982,12 @@
       <c r="E150" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="F150" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="151" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F150" s="3"/>
+      <c r="G150" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="151" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A151" s="3" t="s">
         <v>9</v>
       </c>
@@ -3838,11 +4003,12 @@
       <c r="E151" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="F151" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="152" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F151" s="3"/>
+      <c r="G151" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="152" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A152" s="3" t="s">
         <v>9</v>
       </c>
@@ -3858,11 +4024,12 @@
       <c r="E152" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="F152" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="153" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F152" s="3"/>
+      <c r="G152" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="153" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="3" t="s">
         <v>9</v>
       </c>
@@ -3878,11 +4045,12 @@
       <c r="E153" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="F153" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="154" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F153" s="3"/>
+      <c r="G153" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="154" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="3" t="s">
         <v>9</v>
       </c>
@@ -3898,11 +4066,12 @@
       <c r="E154" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="F154" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="155" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F154" s="3"/>
+      <c r="G154" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="155" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="3" t="s">
         <v>9</v>
       </c>
@@ -3918,11 +4087,12 @@
       <c r="E155" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="F155" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="156" spans="1:6" ht="54" x14ac:dyDescent="0.25">
+      <c r="F155" s="3"/>
+      <c r="G155" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="156" spans="1:7" ht="54" x14ac:dyDescent="0.25">
       <c r="A156" s="3" t="s">
         <v>9</v>
       </c>
@@ -3938,11 +4108,12 @@
       <c r="E156" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="F156" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="157" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F156" s="3"/>
+      <c r="G156" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="157" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="3" t="s">
         <v>9</v>
       </c>
@@ -3958,11 +4129,12 @@
       <c r="E157" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F157" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="158" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F157" s="3"/>
+      <c r="G157" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="158" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A158" s="3" t="s">
         <v>9</v>
       </c>
@@ -3978,11 +4150,12 @@
       <c r="E158" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F158" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="159" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F158" s="3"/>
+      <c r="G158" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="159" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A159" s="3" t="s">
         <v>9</v>
       </c>
@@ -3998,11 +4171,12 @@
       <c r="E159" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F159" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="160" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F159" s="3"/>
+      <c r="G159" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="160" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="3" t="s">
         <v>9</v>
       </c>
@@ -4018,11 +4192,12 @@
       <c r="E160" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F160" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="161" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F160" s="3"/>
+      <c r="G160" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="161" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A161" s="3" t="s">
         <v>9</v>
       </c>
@@ -4038,11 +4213,12 @@
       <c r="E161" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F161" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="162" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F161" s="3"/>
+      <c r="G161" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
         <v>9</v>
       </c>
@@ -4058,11 +4234,12 @@
       <c r="E162" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F162" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="163" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F162" s="3"/>
+      <c r="G162" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
         <v>9</v>
       </c>
@@ -4078,11 +4255,12 @@
       <c r="E163" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="F163" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="164" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F163" s="3"/>
+      <c r="G163" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
         <v>9</v>
       </c>
@@ -4098,11 +4276,12 @@
       <c r="E164" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="F164" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="165" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F164" s="3"/>
+      <c r="G164" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
         <v>9</v>
       </c>
@@ -4118,11 +4297,12 @@
       <c r="E165" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="F165" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="166" spans="1:6" ht="18" x14ac:dyDescent="0.25">
+      <c r="F165" s="3"/>
+      <c r="G165" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
         <v>9</v>
       </c>
@@ -4138,11 +4318,12 @@
       <c r="E166" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F166" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="167" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F166" s="3"/>
+      <c r="G166" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
         <v>9</v>
       </c>
@@ -4158,11 +4339,12 @@
       <c r="E167" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F167" s="3" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="168" spans="1:6" ht="36" x14ac:dyDescent="0.25">
+      <c r="F167" s="3"/>
+      <c r="G167" s="3" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
         <v>9</v>
       </c>
@@ -4178,7 +4360,8 @@
       <c r="E168" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="F168" s="3" t="s">
+      <c r="F168" s="3"/>
+      <c r="G168" s="3" t="s">
         <v>4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
criando servidor único e resolvendo problemas com a api
</commit_message>
<xml_diff>
--- a/database/troubleshooting.xlsx
+++ b/database/troubleshooting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3714512-827F-4250-8959-612905BCC5BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77D47742-7BFB-4A38-AE36-024561F87402}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -809,7 +809,7 @@
   <dimension ref="A1:K168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
preparando resposta com solução
</commit_message>
<xml_diff>
--- a/database/troubleshooting.xlsx
+++ b/database/troubleshooting.xlsx
@@ -5,16 +5,15 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herik\OneDrive\Área de Trabalho\ChatbotSemeq\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A649A32-2CE3-44DA-9822-1869B56FAD9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E30AE5D1-FA07-4F85-90A1-31EED24A4130}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
-    <sheet name="Planilha2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1202" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="177">
   <si>
     <t>interface</t>
   </si>
@@ -373,121 +372,61 @@
     <t>description</t>
   </si>
   <si>
-    <t>Coletor não liga</t>
-  </si>
-  <si>
     <t>Coletor não funciona, Coletor não inicializa, Coletor não acende</t>
   </si>
   <si>
-    <t>Coletor travado</t>
-  </si>
-  <si>
     <t>Coletor não responde, Coletor não se move, Coletor não funciona corretamente</t>
   </si>
   <si>
-    <t>Alerta de ruído ou ausência de sinal</t>
-  </si>
-  <si>
     <t>Alarme de som, Alerta de barulho, Alerta de falta de sinal, Alerta sonoro</t>
   </si>
   <si>
-    <t>Alerta de overload</t>
-  </si>
-  <si>
     <t>Alerta de sobrecarga, Alerta de carga máxima, Alerta de excesso de carga</t>
   </si>
   <si>
-    <t>Alerta de underload</t>
-  </si>
-  <si>
     <t>Alerta de carga mínima, Alerta de carga insuficiente, Alerta de pouca carga</t>
   </si>
   <si>
-    <t>Falha no teclado de membrana</t>
-  </si>
-  <si>
     <t>Teclado não funciona, Teclas não respondem, Teclado não responde corretamente</t>
   </si>
   <si>
-    <t>Problema na conexão internet via Wi-Fi</t>
-  </si>
-  <si>
     <t>Problema de conexão Wi-Fi, Falha na conexão Wi-Fi, Wi-Fi não funciona</t>
   </si>
   <si>
-    <t>Problema na conexão internet via USB</t>
-  </si>
-  <si>
     <t>Problema de conexão USB, Falha na conexão USB, USB não funciona</t>
   </si>
   <si>
-    <t>Não está salvando as medições</t>
-  </si>
-  <si>
     <t>Dados não são salvos, Medições não são salvas, Problema de armazenamento</t>
   </si>
   <si>
-    <t>Equipamento não liga</t>
-  </si>
-  <si>
     <t>Equipamento não funciona, Equipamento não inicializa, Equipamento não acende</t>
   </si>
   <si>
-    <t>Imagem desfocada</t>
-  </si>
-  <si>
     <t>Imagem embaçada, Imagem não nítida, Imagem não focada</t>
   </si>
   <si>
-    <t>Termograma preto</t>
-  </si>
-  <si>
     <t>Imagem termográfica em preto, Termograma sem imagem, Termograma sem leitura</t>
   </si>
   <si>
-    <t>Não salva o termograma</t>
-  </si>
-  <si>
     <t>Termograma não é salvo, Problema de armazenamento de termograma, Dados termográficos não são armazenados</t>
   </si>
   <si>
-    <t>Não carrega a bateria</t>
-  </si>
-  <si>
     <t>Bateria não carrega, Problema de carregamento, Problema na fonte de energia</t>
   </si>
   <si>
-    <t>Câmera liga mas não funciona corretamente</t>
-  </si>
-  <si>
     <t>Problema com a câmera, Câmera não responde, Câmera não grava corretamente</t>
   </si>
   <si>
-    <t>Câmera embaçada ou vídeos lavados</t>
-  </si>
-  <si>
     <t>Imagem da câmera desfocada, Vídeos da câmera sem qualidade, Vídeos da câmera não nítidos</t>
   </si>
   <si>
-    <t>Câmera não se conecta no USB</t>
-  </si>
-  <si>
     <t>Problema de conexão USB da câmera, Falha na conexão USB da câmera, Câmera não se comunica com o computador</t>
   </si>
   <si>
-    <t>Câmera não segura carga</t>
-  </si>
-  <si>
     <t>Bateria da câmera não dura, Problema de bateria da câmera, Câmera não segura carga</t>
   </si>
   <si>
-    <t>Bateria baixa</t>
-  </si>
-  <si>
     <t>Pouca carga na bateria, Bateria descarregando, Bateria fraca</t>
-  </si>
-  <si>
-    <t>Não lê corrente</t>
   </si>
   <si>
     <t>Problema de leitura de corrente, Falha na leitura de corrente, Corrente não é lida</t>
@@ -1105,7 +1044,7 @@
   <dimension ref="A1:K168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1147,7 +1086,7 @@
     </row>
     <row r="2" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1162,7 +1101,7 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>4</v>
@@ -1172,7 +1111,7 @@
     </row>
     <row r="3" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1187,7 +1126,7 @@
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>4</v>
@@ -1197,7 +1136,7 @@
     </row>
     <row r="4" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1212,7 +1151,7 @@
         <v>13</v>
       </c>
       <c r="F4" s="2" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="G4" s="2" t="s">
         <v>4</v>
@@ -1222,7 +1161,7 @@
     </row>
     <row r="5" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -1237,7 +1176,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>4</v>
@@ -1248,7 +1187,7 @@
     </row>
     <row r="6" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -1263,7 +1202,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>4</v>
@@ -1273,7 +1212,7 @@
     </row>
     <row r="7" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -1288,7 +1227,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>4</v>
@@ -1298,7 +1237,7 @@
     </row>
     <row r="8" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -1313,7 +1252,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>4</v>
@@ -1323,7 +1262,7 @@
     </row>
     <row r="9" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -1338,7 +1277,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>130</v>
+        <v>122</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>4</v>
@@ -1348,7 +1287,7 @@
     </row>
     <row r="10" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -1363,7 +1302,7 @@
         <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>4</v>
@@ -1373,7 +1312,7 @@
     </row>
     <row r="11" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -1388,7 +1327,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>4</v>
@@ -1398,7 +1337,7 @@
     </row>
     <row r="12" spans="1:11" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
@@ -1413,7 +1352,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>4</v>
@@ -1423,7 +1362,7 @@
     </row>
     <row r="13" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -1438,7 +1377,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>4</v>
@@ -1448,7 +1387,7 @@
     </row>
     <row r="14" spans="1:11" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>8</v>
@@ -1463,7 +1402,7 @@
         <v>25</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>4</v>
@@ -1473,7 +1412,7 @@
     </row>
     <row r="15" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -1488,7 +1427,7 @@
         <v>26</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>4</v>
@@ -1498,7 +1437,7 @@
     </row>
     <row r="16" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -1513,7 +1452,7 @@
         <v>27</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>4</v>
@@ -1523,7 +1462,7 @@
     </row>
     <row r="17" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -1538,7 +1477,7 @@
         <v>28</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>4</v>
@@ -1548,7 +1487,7 @@
     </row>
     <row r="18" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>8</v>
@@ -1563,7 +1502,7 @@
         <v>29</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>4</v>
@@ -1573,7 +1512,7 @@
     </row>
     <row r="19" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>8</v>
@@ -1588,7 +1527,7 @@
         <v>30</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>4</v>
@@ -1598,7 +1537,7 @@
     </row>
     <row r="20" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>8</v>
@@ -1613,7 +1552,7 @@
         <v>22</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>134</v>
+        <v>124</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>4</v>
@@ -1623,7 +1562,7 @@
     </row>
     <row r="21" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
@@ -1638,7 +1577,7 @@
         <v>23</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>4</v>
@@ -1648,7 +1587,7 @@
     </row>
     <row r="22" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
@@ -1663,7 +1602,7 @@
         <v>24</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>138</v>
+        <v>126</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>4</v>
@@ -1671,7 +1610,7 @@
     </row>
     <row r="23" spans="1:11" ht="108" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
@@ -1686,7 +1625,7 @@
         <v>25</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>140</v>
+        <v>127</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>4</v>
@@ -1694,7 +1633,7 @@
     </row>
     <row r="24" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
@@ -1709,7 +1648,7 @@
         <v>26</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>4</v>
@@ -1717,7 +1656,7 @@
     </row>
     <row r="25" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>8</v>
@@ -1732,7 +1671,7 @@
         <v>27</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>144</v>
+        <v>129</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>4</v>
@@ -1740,7 +1679,7 @@
     </row>
     <row r="26" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>8</v>
@@ -1755,7 +1694,7 @@
         <v>28</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>146</v>
+        <v>130</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>4</v>
@@ -1763,7 +1702,7 @@
     </row>
     <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
@@ -1778,7 +1717,7 @@
         <v>29</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>148</v>
+        <v>131</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>4</v>
@@ -1786,7 +1725,7 @@
     </row>
     <row r="28" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
@@ -1801,7 +1740,7 @@
         <v>30</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>150</v>
+        <v>132</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>4</v>
@@ -1809,7 +1748,7 @@
     </row>
     <row r="29" spans="1:11" ht="54" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
@@ -1824,7 +1763,7 @@
         <v>34</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>152</v>
+        <v>133</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>4</v>
@@ -1832,7 +1771,7 @@
     </row>
     <row r="30" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>196</v>
+        <v>176</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
@@ -1847,7 +1786,7 @@
         <v>35</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>4</v>
@@ -1870,7 +1809,7 @@
         <v>39</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>4</v>
@@ -1895,7 +1834,7 @@
         <v>40</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>4</v>
@@ -1920,7 +1859,7 @@
         <v>39</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>4</v>
@@ -1945,7 +1884,7 @@
         <v>40</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>4</v>
@@ -1970,7 +1909,7 @@
         <v>39</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>155</v>
+        <v>135</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>4</v>
@@ -1995,7 +1934,7 @@
         <v>40</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>4</v>
@@ -2020,7 +1959,7 @@
         <v>48</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>4</v>
@@ -2045,7 +1984,7 @@
         <v>48</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>4</v>
@@ -2070,7 +2009,7 @@
         <v>48</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>4</v>
@@ -2095,7 +2034,7 @@
         <v>48</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>4</v>
@@ -2120,7 +2059,7 @@
         <v>48</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>4</v>
@@ -2145,7 +2084,7 @@
         <v>48</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>4</v>
@@ -2170,7 +2109,7 @@
         <v>48</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>4</v>
@@ -2195,7 +2134,7 @@
         <v>48</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>4</v>
@@ -2220,7 +2159,7 @@
         <v>48</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>4</v>
@@ -2245,7 +2184,7 @@
         <v>48</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>4</v>
@@ -2270,7 +2209,7 @@
         <v>58</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>4</v>
@@ -2295,7 +2234,7 @@
         <v>60</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>4</v>
@@ -2320,7 +2259,7 @@
         <v>62</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>4</v>
@@ -2345,7 +2284,7 @@
         <v>62</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>4</v>
@@ -2370,7 +2309,7 @@
         <v>65</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>4</v>
@@ -2395,7 +2334,7 @@
         <v>66</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>4</v>
@@ -2420,7 +2359,7 @@
         <v>67</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>4</v>
@@ -2445,7 +2384,7 @@
         <v>68</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>4</v>
@@ -2470,7 +2409,7 @@
         <v>69</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>4</v>
@@ -2495,7 +2434,7 @@
         <v>70</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>4</v>
@@ -2518,7 +2457,7 @@
         <v>71</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>4</v>
@@ -2541,7 +2480,7 @@
         <v>72</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>4</v>
@@ -2564,7 +2503,7 @@
         <v>73</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>4</v>
@@ -2587,7 +2526,7 @@
         <v>65</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>4</v>
@@ -2610,7 +2549,7 @@
         <v>66</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>4</v>
@@ -2633,7 +2572,7 @@
         <v>67</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>4</v>
@@ -2656,7 +2595,7 @@
         <v>68</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>4</v>
@@ -2679,7 +2618,7 @@
         <v>69</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>4</v>
@@ -2702,7 +2641,7 @@
         <v>70</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>4</v>
@@ -2725,7 +2664,7 @@
         <v>71</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>4</v>
@@ -2748,7 +2687,7 @@
         <v>72</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>4</v>
@@ -2771,7 +2710,7 @@
         <v>73</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>4</v>
@@ -2794,7 +2733,7 @@
         <v>76</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>4</v>
@@ -2817,7 +2756,7 @@
         <v>76</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>4</v>
@@ -2840,7 +2779,7 @@
         <v>77</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>4</v>
@@ -2863,7 +2802,7 @@
         <v>79</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>4</v>
@@ -2886,7 +2825,7 @@
         <v>79</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>4</v>
@@ -2909,7 +2848,7 @@
         <v>82</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>4</v>
@@ -2932,7 +2871,7 @@
         <v>83</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>4</v>
@@ -2955,7 +2894,7 @@
         <v>86</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>4</v>
@@ -2978,7 +2917,7 @@
         <v>83</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>4</v>
@@ -3001,7 +2940,7 @@
         <v>89</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>4</v>
@@ -3024,7 +2963,7 @@
         <v>90</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>4</v>
@@ -3047,7 +2986,7 @@
         <v>91</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>4</v>
@@ -3070,7 +3009,7 @@
         <v>89</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>4</v>
@@ -3093,7 +3032,7 @@
         <v>90</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>4</v>
@@ -3116,7 +3055,7 @@
         <v>91</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>4</v>
@@ -3139,7 +3078,7 @@
         <v>89</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>4</v>
@@ -3162,7 +3101,7 @@
         <v>90</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>4</v>
@@ -3185,7 +3124,7 @@
         <v>91</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>4</v>
@@ -3208,7 +3147,7 @@
         <v>95</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>4</v>
@@ -3231,7 +3170,7 @@
         <v>58</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>158</v>
+        <v>138</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>4</v>
@@ -3254,7 +3193,7 @@
         <v>60</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>159</v>
+        <v>139</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>4</v>
@@ -3277,7 +3216,7 @@
         <v>62</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>4</v>
@@ -3300,7 +3239,7 @@
         <v>62</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>160</v>
+        <v>140</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>4</v>
@@ -3323,7 +3262,7 @@
         <v>65</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>4</v>
@@ -3346,7 +3285,7 @@
         <v>66</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>4</v>
@@ -3369,7 +3308,7 @@
         <v>67</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>4</v>
@@ -3392,7 +3331,7 @@
         <v>68</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>4</v>
@@ -3415,7 +3354,7 @@
         <v>69</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>4</v>
@@ -3438,7 +3377,7 @@
         <v>70</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>4</v>
@@ -3461,7 +3400,7 @@
         <v>71</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>4</v>
@@ -3484,7 +3423,7 @@
         <v>72</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>4</v>
@@ -3507,7 +3446,7 @@
         <v>73</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>4</v>
@@ -3530,7 +3469,7 @@
         <v>65</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>161</v>
+        <v>141</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>4</v>
@@ -3553,7 +3492,7 @@
         <v>66</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>162</v>
+        <v>142</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>4</v>
@@ -3576,7 +3515,7 @@
         <v>67</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>163</v>
+        <v>143</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>4</v>
@@ -3599,7 +3538,7 @@
         <v>68</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>164</v>
+        <v>144</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>4</v>
@@ -3622,7 +3561,7 @@
         <v>69</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>165</v>
+        <v>145</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>4</v>
@@ -3645,7 +3584,7 @@
         <v>70</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>166</v>
+        <v>146</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>4</v>
@@ -3668,7 +3607,7 @@
         <v>71</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>167</v>
+        <v>147</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>4</v>
@@ -3691,7 +3630,7 @@
         <v>72</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>168</v>
+        <v>148</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>4</v>
@@ -3714,7 +3653,7 @@
         <v>73</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>169</v>
+        <v>149</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>4</v>
@@ -3737,7 +3676,7 @@
         <v>76</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>4</v>
@@ -3760,7 +3699,7 @@
         <v>76</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>170</v>
+        <v>150</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>4</v>
@@ -3783,7 +3722,7 @@
         <v>77</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>171</v>
+        <v>151</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>4</v>
@@ -3806,7 +3745,7 @@
         <v>79</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>4</v>
@@ -3829,7 +3768,7 @@
         <v>79</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>172</v>
+        <v>152</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>4</v>
@@ -3852,7 +3791,7 @@
         <v>82</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>173</v>
+        <v>153</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>4</v>
@@ -3875,7 +3814,7 @@
         <v>83</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>4</v>
@@ -3898,7 +3837,7 @@
         <v>86</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>175</v>
+        <v>155</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>4</v>
@@ -3921,7 +3860,7 @@
         <v>83</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>174</v>
+        <v>154</v>
       </c>
       <c r="G118" s="2" t="s">
         <v>4</v>
@@ -3944,7 +3883,7 @@
         <v>89</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>4</v>
@@ -3967,7 +3906,7 @@
         <v>90</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>4</v>
@@ -3990,7 +3929,7 @@
         <v>91</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>4</v>
@@ -4013,7 +3952,7 @@
         <v>89</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>4</v>
@@ -4036,7 +3975,7 @@
         <v>90</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>4</v>
@@ -4059,7 +3998,7 @@
         <v>91</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>4</v>
@@ -4082,7 +4021,7 @@
         <v>89</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>176</v>
+        <v>156</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>4</v>
@@ -4105,7 +4044,7 @@
         <v>90</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>4</v>
@@ -4128,7 +4067,7 @@
         <v>91</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>178</v>
+        <v>158</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>4</v>
@@ -4151,7 +4090,7 @@
         <v>95</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>179</v>
+        <v>159</v>
       </c>
       <c r="G128" s="2" t="s">
         <v>4</v>
@@ -4174,7 +4113,7 @@
         <v>65</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="G129" s="2" t="s">
         <v>4</v>
@@ -4199,7 +4138,7 @@
         <v>66</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="G130" s="2" t="s">
         <v>4</v>
@@ -4224,7 +4163,7 @@
         <v>67</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="G131" s="2" t="s">
         <v>4</v>
@@ -4249,7 +4188,7 @@
         <v>68</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="G132" s="2" t="s">
         <v>4</v>
@@ -4274,7 +4213,7 @@
         <v>69</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>4</v>
@@ -4299,7 +4238,7 @@
         <v>70</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>4</v>
@@ -4324,7 +4263,7 @@
         <v>71</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>4</v>
@@ -4349,7 +4288,7 @@
         <v>72</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>4</v>
@@ -4374,7 +4313,7 @@
         <v>73</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="G137" s="2" t="s">
         <v>4</v>
@@ -4399,7 +4338,7 @@
         <v>65</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>4</v>
@@ -4424,7 +4363,7 @@
         <v>66</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>4</v>
@@ -4449,7 +4388,7 @@
         <v>67</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="G140" s="2" t="s">
         <v>4</v>
@@ -4474,7 +4413,7 @@
         <v>68</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="G141" s="2" t="s">
         <v>4</v>
@@ -4499,7 +4438,7 @@
         <v>69</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="G142" s="2" t="s">
         <v>4</v>
@@ -4524,7 +4463,7 @@
         <v>70</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="G143" s="2" t="s">
         <v>4</v>
@@ -4549,7 +4488,7 @@
         <v>71</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>4</v>
@@ -4574,7 +4513,7 @@
         <v>72</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>4</v>
@@ -4597,7 +4536,7 @@
         <v>73</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>4</v>
@@ -4620,7 +4559,7 @@
         <v>65</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>4</v>
@@ -4643,7 +4582,7 @@
         <v>66</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>181</v>
+        <v>161</v>
       </c>
       <c r="G148" s="2" t="s">
         <v>4</v>
@@ -4666,7 +4605,7 @@
         <v>67</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>182</v>
+        <v>162</v>
       </c>
       <c r="G149" s="2" t="s">
         <v>4</v>
@@ -4689,7 +4628,7 @@
         <v>68</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>183</v>
+        <v>163</v>
       </c>
       <c r="G150" s="2" t="s">
         <v>4</v>
@@ -4712,7 +4651,7 @@
         <v>69</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>184</v>
+        <v>164</v>
       </c>
       <c r="G151" s="2" t="s">
         <v>4</v>
@@ -4735,7 +4674,7 @@
         <v>70</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>185</v>
+        <v>165</v>
       </c>
       <c r="G152" s="2" t="s">
         <v>4</v>
@@ -4758,7 +4697,7 @@
         <v>71</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>186</v>
+        <v>166</v>
       </c>
       <c r="G153" s="2" t="s">
         <v>4</v>
@@ -4781,7 +4720,7 @@
         <v>72</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>187</v>
+        <v>167</v>
       </c>
       <c r="G154" s="2" t="s">
         <v>4</v>
@@ -4804,7 +4743,7 @@
         <v>73</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>188</v>
+        <v>168</v>
       </c>
       <c r="G155" s="2" t="s">
         <v>4</v>
@@ -4827,7 +4766,7 @@
         <v>103</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>189</v>
+        <v>169</v>
       </c>
       <c r="G156" s="2" t="s">
         <v>4</v>
@@ -4850,7 +4789,7 @@
         <v>106</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="G157" s="2" t="s">
         <v>4</v>
@@ -4873,7 +4812,7 @@
         <v>107</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="G158" s="2" t="s">
         <v>4</v>
@@ -4896,7 +4835,7 @@
         <v>108</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="G159" s="2" t="s">
         <v>4</v>
@@ -4919,7 +4858,7 @@
         <v>109</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="G160" s="2" t="s">
         <v>4</v>
@@ -4942,7 +4881,7 @@
         <v>110</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="G161" s="2" t="s">
         <v>4</v>
@@ -4965,7 +4904,7 @@
         <v>111</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="G162" s="2" t="s">
         <v>4</v>
@@ -4988,7 +4927,7 @@
         <v>106</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>190</v>
+        <v>170</v>
       </c>
       <c r="G163" s="2" t="s">
         <v>4</v>
@@ -5011,7 +4950,7 @@
         <v>107</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>191</v>
+        <v>171</v>
       </c>
       <c r="G164" s="2" t="s">
         <v>4</v>
@@ -5034,7 +4973,7 @@
         <v>108</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>192</v>
+        <v>172</v>
       </c>
       <c r="G165" s="2" t="s">
         <v>4</v>
@@ -5057,7 +4996,7 @@
         <v>109</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>193</v>
+        <v>173</v>
       </c>
       <c r="G166" s="2" t="s">
         <v>4</v>
@@ -5080,7 +5019,7 @@
         <v>110</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>194</v>
+        <v>174</v>
       </c>
       <c r="G167" s="2" t="s">
         <v>4</v>
@@ -5103,7 +5042,7 @@
         <v>111</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>195</v>
+        <v>175</v>
       </c>
       <c r="G168" s="2" t="s">
         <v>4</v>
@@ -5114,183 +5053,4 @@
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3255211E-AF48-4A1C-BD9E-C4AF2D96FF97}">
-  <dimension ref="A1:B20"/>
-  <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B20" sqref="A1:B20"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="33.28515625" customWidth="1"/>
-    <col min="2" max="2" width="51" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="B1" s="4" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="3" t="s">
-        <v>119</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>120</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>124</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>125</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="3" t="s">
-        <v>139</v>
-      </c>
-      <c r="B13" s="4" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="3" t="s">
-        <v>141</v>
-      </c>
-      <c r="B14" s="4" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>143</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>145</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>154</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
finalizando tela de apresentação
</commit_message>
<xml_diff>
--- a/database/troubleshooting.xlsx
+++ b/database/troubleshooting.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\herik\OneDrive\Área de Trabalho\ChatbotSemeq\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABB45C12-8D71-4F31-9284-129F0A61B51B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{22F0CDDA-A2DC-4FB4-A001-F18F7318C5C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="177">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="178">
   <si>
     <t>interface</t>
   </si>
@@ -381,9 +381,6 @@
     <t>Alarme de som, Alerta de barulho, Alerta de falta de sinal, Alerta sonoro</t>
   </si>
   <si>
-    <t>Alerta de sobrecarga, Alerta de carga máxima, Alerta de excesso de carga</t>
-  </si>
-  <si>
     <t>Alerta de carga mínima, Alerta de carga insuficiente, Alerta de pouca carga</t>
   </si>
   <si>
@@ -556,6 +553,12 @@
   </si>
   <si>
     <t>coleta periodica offline</t>
+  </si>
+  <si>
+    <t>Alerta de sobrecarga, Alerta de carga máxima, Alerta de excesso de carga,coletor está com alerta de sobrecarga,coletor está com alerta de overload</t>
+  </si>
+  <si>
+    <t>Falha ao carregar priorização, priorização do mysemeq não carrega</t>
   </si>
 </sst>
 </file>
@@ -1043,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E221B1-E974-48EE-8D2F-4D47A5EBE7F7}">
   <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F33" sqref="F33"/>
+    <sheetView tabSelected="1" topLeftCell="A40" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="I58" sqref="I58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1086,7 +1089,7 @@
     </row>
     <row r="2" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1111,7 +1114,7 @@
     </row>
     <row r="3" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1136,7 +1139,7 @@
     </row>
     <row r="4" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1159,9 +1162,9 @@
       <c r="J4" s="3"/>
       <c r="K4" s="4"/>
     </row>
-    <row r="5" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -1176,7 +1179,7 @@
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>118</v>
+        <v>176</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>4</v>
@@ -1187,7 +1190,7 @@
     </row>
     <row r="6" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -1202,7 +1205,7 @@
         <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>4</v>
@@ -1212,7 +1215,7 @@
     </row>
     <row r="7" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -1227,7 +1230,7 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>4</v>
@@ -1237,7 +1240,7 @@
     </row>
     <row r="8" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -1252,7 +1255,7 @@
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>4</v>
@@ -1262,7 +1265,7 @@
     </row>
     <row r="9" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -1277,7 +1280,7 @@
         <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>4</v>
@@ -1287,7 +1290,7 @@
     </row>
     <row r="10" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -1302,7 +1305,7 @@
         <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>4</v>
@@ -1312,7 +1315,7 @@
     </row>
     <row r="11" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -1327,7 +1330,7 @@
         <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>4</v>
@@ -1337,7 +1340,7 @@
     </row>
     <row r="12" spans="1:11" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
@@ -1352,7 +1355,7 @@
         <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>4</v>
@@ -1362,7 +1365,7 @@
     </row>
     <row r="13" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -1377,7 +1380,7 @@
         <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>4</v>
@@ -1387,7 +1390,7 @@
     </row>
     <row r="14" spans="1:11" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>8</v>
@@ -1402,7 +1405,7 @@
         <v>25</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>4</v>
@@ -1412,7 +1415,7 @@
     </row>
     <row r="15" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -1427,7 +1430,7 @@
         <v>26</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>4</v>
@@ -1437,7 +1440,7 @@
     </row>
     <row r="16" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -1452,7 +1455,7 @@
         <v>27</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>4</v>
@@ -1462,7 +1465,7 @@
     </row>
     <row r="17" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -1477,7 +1480,7 @@
         <v>28</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>4</v>
@@ -1487,7 +1490,7 @@
     </row>
     <row r="18" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>8</v>
@@ -1502,7 +1505,7 @@
         <v>29</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>4</v>
@@ -1512,7 +1515,7 @@
     </row>
     <row r="19" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>8</v>
@@ -1527,7 +1530,7 @@
         <v>30</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>4</v>
@@ -1537,7 +1540,7 @@
     </row>
     <row r="20" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>8</v>
@@ -1552,7 +1555,7 @@
         <v>22</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>4</v>
@@ -1562,7 +1565,7 @@
     </row>
     <row r="21" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
@@ -1577,7 +1580,7 @@
         <v>23</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>4</v>
@@ -1587,7 +1590,7 @@
     </row>
     <row r="22" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
@@ -1602,7 +1605,7 @@
         <v>24</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>4</v>
@@ -1610,7 +1613,7 @@
     </row>
     <row r="23" spans="1:11" ht="108" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
@@ -1625,7 +1628,7 @@
         <v>25</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>4</v>
@@ -1633,7 +1636,7 @@
     </row>
     <row r="24" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
@@ -1648,7 +1651,7 @@
         <v>26</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>4</v>
@@ -1656,7 +1659,7 @@
     </row>
     <row r="25" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>8</v>
@@ -1671,7 +1674,7 @@
         <v>27</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>4</v>
@@ -1679,7 +1682,7 @@
     </row>
     <row r="26" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>8</v>
@@ -1694,7 +1697,7 @@
         <v>28</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>4</v>
@@ -1702,7 +1705,7 @@
     </row>
     <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
@@ -1717,7 +1720,7 @@
         <v>29</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>4</v>
@@ -1725,7 +1728,7 @@
     </row>
     <row r="28" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
@@ -1740,7 +1743,7 @@
         <v>30</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>4</v>
@@ -1748,7 +1751,7 @@
     </row>
     <row r="29" spans="1:11" ht="54" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
@@ -1763,7 +1766,7 @@
         <v>34</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>4</v>
@@ -1771,7 +1774,7 @@
     </row>
     <row r="30" spans="1:11" ht="72" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
@@ -1786,7 +1789,7 @@
         <v>35</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>4</v>
@@ -1809,7 +1812,7 @@
         <v>39</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>4</v>
@@ -1834,7 +1837,7 @@
         <v>40</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>4</v>
@@ -1859,7 +1862,7 @@
         <v>39</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>4</v>
@@ -1884,7 +1887,7 @@
         <v>40</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>4</v>
@@ -1909,7 +1912,7 @@
         <v>39</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>4</v>
@@ -1934,7 +1937,7 @@
         <v>40</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>4</v>
@@ -1959,7 +1962,7 @@
         <v>48</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>4</v>
@@ -1984,7 +1987,7 @@
         <v>48</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>4</v>
@@ -2009,7 +2012,7 @@
         <v>48</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>4</v>
@@ -2034,7 +2037,7 @@
         <v>48</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>4</v>
@@ -2059,7 +2062,7 @@
         <v>48</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>4</v>
@@ -2084,7 +2087,7 @@
         <v>48</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>4</v>
@@ -2109,7 +2112,7 @@
         <v>48</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>4</v>
@@ -2134,7 +2137,7 @@
         <v>48</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>4</v>
@@ -2159,7 +2162,7 @@
         <v>48</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>4</v>
@@ -2184,7 +2187,7 @@
         <v>48</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>4</v>
@@ -2209,7 +2212,7 @@
         <v>58</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>4</v>
@@ -2234,7 +2237,7 @@
         <v>60</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>4</v>
@@ -2259,7 +2262,7 @@
         <v>62</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>4</v>
@@ -2284,7 +2287,7 @@
         <v>62</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>4</v>
@@ -2309,7 +2312,7 @@
         <v>65</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>4</v>
@@ -2334,7 +2337,7 @@
         <v>66</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>4</v>
@@ -2359,7 +2362,7 @@
         <v>67</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>4</v>
@@ -2384,7 +2387,7 @@
         <v>68</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>4</v>
@@ -2409,7 +2412,7 @@
         <v>69</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>4</v>
@@ -2434,7 +2437,7 @@
         <v>70</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>4</v>
@@ -2457,7 +2460,7 @@
         <v>71</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>4</v>
@@ -2480,13 +2483,13 @@
         <v>72</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="36" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="54" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>54</v>
       </c>
@@ -2503,7 +2506,7 @@
         <v>73</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>4</v>
@@ -2526,7 +2529,7 @@
         <v>65</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>4</v>
@@ -2549,7 +2552,7 @@
         <v>66</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>4</v>
@@ -2572,7 +2575,7 @@
         <v>67</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>4</v>
@@ -2595,7 +2598,7 @@
         <v>68</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>4</v>
@@ -2618,7 +2621,7 @@
         <v>69</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>4</v>
@@ -2641,7 +2644,7 @@
         <v>70</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>4</v>
@@ -2664,7 +2667,7 @@
         <v>71</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>4</v>
@@ -2687,7 +2690,7 @@
         <v>72</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>4</v>
@@ -2710,7 +2713,7 @@
         <v>73</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>4</v>
@@ -2733,7 +2736,7 @@
         <v>76</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>4</v>
@@ -2756,7 +2759,7 @@
         <v>76</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>4</v>
@@ -2779,7 +2782,7 @@
         <v>77</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>4</v>
@@ -2802,7 +2805,7 @@
         <v>79</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>4</v>
@@ -2825,7 +2828,7 @@
         <v>79</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>4</v>
@@ -2848,7 +2851,7 @@
         <v>82</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>4</v>
@@ -2871,7 +2874,7 @@
         <v>83</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>4</v>
@@ -2894,7 +2897,7 @@
         <v>86</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>4</v>
@@ -2917,7 +2920,7 @@
         <v>83</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>4</v>
@@ -2940,7 +2943,7 @@
         <v>89</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>4</v>
@@ -2963,7 +2966,7 @@
         <v>90</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>4</v>
@@ -2986,7 +2989,7 @@
         <v>91</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>4</v>
@@ -3009,7 +3012,7 @@
         <v>89</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>4</v>
@@ -3032,7 +3035,7 @@
         <v>90</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>4</v>
@@ -3055,7 +3058,7 @@
         <v>91</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>4</v>
@@ -3078,7 +3081,7 @@
         <v>89</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>4</v>
@@ -3101,7 +3104,7 @@
         <v>90</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>4</v>
@@ -3124,7 +3127,7 @@
         <v>91</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>4</v>
@@ -3147,7 +3150,7 @@
         <v>95</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>4</v>
@@ -3170,7 +3173,7 @@
         <v>58</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>4</v>
@@ -3193,7 +3196,7 @@
         <v>60</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>4</v>
@@ -3216,7 +3219,7 @@
         <v>62</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>4</v>
@@ -3239,7 +3242,7 @@
         <v>62</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>4</v>
@@ -3262,7 +3265,7 @@
         <v>65</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>4</v>
@@ -3285,7 +3288,7 @@
         <v>66</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>4</v>
@@ -3308,7 +3311,7 @@
         <v>67</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>4</v>
@@ -3331,7 +3334,7 @@
         <v>68</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>4</v>
@@ -3354,7 +3357,7 @@
         <v>69</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>4</v>
@@ -3377,7 +3380,7 @@
         <v>70</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>4</v>
@@ -3400,7 +3403,7 @@
         <v>71</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>4</v>
@@ -3423,7 +3426,7 @@
         <v>72</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>4</v>
@@ -3446,7 +3449,7 @@
         <v>73</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>4</v>
@@ -3469,7 +3472,7 @@
         <v>65</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>4</v>
@@ -3492,7 +3495,7 @@
         <v>66</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>4</v>
@@ -3515,7 +3518,7 @@
         <v>67</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>4</v>
@@ -3538,7 +3541,7 @@
         <v>68</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>4</v>
@@ -3561,7 +3564,7 @@
         <v>69</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>4</v>
@@ -3584,7 +3587,7 @@
         <v>70</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>4</v>
@@ -3607,7 +3610,7 @@
         <v>71</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>4</v>
@@ -3630,7 +3633,7 @@
         <v>72</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>4</v>
@@ -3653,7 +3656,7 @@
         <v>73</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>4</v>
@@ -3676,7 +3679,7 @@
         <v>76</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>4</v>
@@ -3699,7 +3702,7 @@
         <v>76</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>4</v>
@@ -3722,7 +3725,7 @@
         <v>77</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>4</v>
@@ -3745,7 +3748,7 @@
         <v>79</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>4</v>
@@ -3768,7 +3771,7 @@
         <v>79</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>4</v>
@@ -3791,7 +3794,7 @@
         <v>82</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>4</v>
@@ -3814,7 +3817,7 @@
         <v>83</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>4</v>
@@ -3837,7 +3840,7 @@
         <v>86</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>4</v>
@@ -3860,7 +3863,7 @@
         <v>83</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="G118" s="2" t="s">
         <v>4</v>
@@ -3883,7 +3886,7 @@
         <v>89</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>4</v>
@@ -3906,7 +3909,7 @@
         <v>90</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>4</v>
@@ -3929,7 +3932,7 @@
         <v>91</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>4</v>
@@ -3952,7 +3955,7 @@
         <v>89</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>4</v>
@@ -3975,7 +3978,7 @@
         <v>90</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>4</v>
@@ -3998,7 +4001,7 @@
         <v>91</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>4</v>
@@ -4021,7 +4024,7 @@
         <v>89</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>4</v>
@@ -4044,7 +4047,7 @@
         <v>90</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>4</v>
@@ -4067,7 +4070,7 @@
         <v>91</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>4</v>
@@ -4090,7 +4093,7 @@
         <v>95</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="G128" s="2" t="s">
         <v>4</v>
@@ -4113,7 +4116,7 @@
         <v>65</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G129" s="2" t="s">
         <v>4</v>
@@ -4138,7 +4141,7 @@
         <v>66</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G130" s="2" t="s">
         <v>4</v>
@@ -4163,7 +4166,7 @@
         <v>67</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G131" s="2" t="s">
         <v>4</v>
@@ -4188,7 +4191,7 @@
         <v>68</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G132" s="2" t="s">
         <v>4</v>
@@ -4213,7 +4216,7 @@
         <v>69</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>4</v>
@@ -4238,7 +4241,7 @@
         <v>70</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>4</v>
@@ -4263,7 +4266,7 @@
         <v>71</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>4</v>
@@ -4288,7 +4291,7 @@
         <v>72</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>4</v>
@@ -4313,7 +4316,7 @@
         <v>73</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G137" s="2" t="s">
         <v>4</v>
@@ -4338,7 +4341,7 @@
         <v>65</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>4</v>
@@ -4363,7 +4366,7 @@
         <v>66</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>4</v>
@@ -4388,7 +4391,7 @@
         <v>67</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G140" s="2" t="s">
         <v>4</v>
@@ -4413,7 +4416,7 @@
         <v>68</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G141" s="2" t="s">
         <v>4</v>
@@ -4438,7 +4441,7 @@
         <v>69</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G142" s="2" t="s">
         <v>4</v>
@@ -4463,7 +4466,7 @@
         <v>70</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G143" s="2" t="s">
         <v>4</v>
@@ -4488,7 +4491,7 @@
         <v>71</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>4</v>
@@ -4513,7 +4516,7 @@
         <v>72</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>4</v>
@@ -4536,7 +4539,7 @@
         <v>73</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>4</v>
@@ -4559,7 +4562,7 @@
         <v>65</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>4</v>
@@ -4582,7 +4585,7 @@
         <v>66</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="G148" s="2" t="s">
         <v>4</v>
@@ -4605,7 +4608,7 @@
         <v>67</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="G149" s="2" t="s">
         <v>4</v>
@@ -4628,7 +4631,7 @@
         <v>68</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="G150" s="2" t="s">
         <v>4</v>
@@ -4651,7 +4654,7 @@
         <v>69</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="G151" s="2" t="s">
         <v>4</v>
@@ -4674,7 +4677,7 @@
         <v>70</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="G152" s="2" t="s">
         <v>4</v>
@@ -4697,7 +4700,7 @@
         <v>71</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="G153" s="2" t="s">
         <v>4</v>
@@ -4720,7 +4723,7 @@
         <v>72</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="G154" s="2" t="s">
         <v>4</v>
@@ -4743,7 +4746,7 @@
         <v>73</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="G155" s="2" t="s">
         <v>4</v>
@@ -4766,7 +4769,7 @@
         <v>103</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G156" s="2" t="s">
         <v>4</v>
@@ -4789,7 +4792,7 @@
         <v>106</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G157" s="2" t="s">
         <v>4</v>
@@ -4812,7 +4815,7 @@
         <v>107</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G158" s="2" t="s">
         <v>4</v>
@@ -4835,7 +4838,7 @@
         <v>108</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G159" s="2" t="s">
         <v>4</v>
@@ -4858,7 +4861,7 @@
         <v>109</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G160" s="2" t="s">
         <v>4</v>
@@ -4881,7 +4884,7 @@
         <v>110</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G161" s="2" t="s">
         <v>4</v>
@@ -4904,7 +4907,7 @@
         <v>111</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G162" s="2" t="s">
         <v>4</v>
@@ -4927,7 +4930,7 @@
         <v>106</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="G163" s="2" t="s">
         <v>4</v>
@@ -4950,7 +4953,7 @@
         <v>107</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G164" s="2" t="s">
         <v>4</v>
@@ -4973,7 +4976,7 @@
         <v>108</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="G165" s="2" t="s">
         <v>4</v>
@@ -4996,7 +4999,7 @@
         <v>109</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="G166" s="2" t="s">
         <v>4</v>
@@ -5019,7 +5022,7 @@
         <v>110</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="G167" s="2" t="s">
         <v>4</v>
@@ -5042,7 +5045,7 @@
         <v>111</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G168" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
criando e modelando o banco de dados em sqlite
</commit_message>
<xml_diff>
--- a/database/troubleshooting.xlsx
+++ b/database/troubleshooting.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C69A93C-CD3F-4EE6-B1DD-712071BAE2B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131708C2-B7D2-41B4-9FB7-3A265A84C589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
+    <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -1047,7 +1047,7 @@
   <dimension ref="A1:K168"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F59" sqref="F59"/>
+      <selection activeCell="E1" sqref="E1:E30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
função de tf e idf pronta
</commit_message>
<xml_diff>
--- a/database/troubleshooting.xlsx
+++ b/database/troubleshooting.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{131708C2-B7D2-41B4-9FB7-3A265A84C589}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BCC759-C4A2-43E1-9791-3F16ECF6EAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
   </bookViews>
@@ -1046,8 +1046,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E221B1-E974-48EE-8D2F-4D47A5EBE7F7}">
   <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E1" sqref="E1:E30"/>
+    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
estudando formas de otimizar o preprocessamento
</commit_message>
<xml_diff>
--- a/database/troubleshooting.xlsx
+++ b/database/troubleshooting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47BCC759-C4A2-43E1-9791-3F16ECF6EAFF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{798E4115-6BD0-4BBB-9757-D6C809615E9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1162" uniqueCount="189">
   <si>
     <t>interface</t>
   </si>
@@ -372,200 +372,233 @@
     <t>description</t>
   </si>
   <si>
-    <t>Coletor não funciona, Coletor não inicializa, Coletor não acende</t>
-  </si>
-  <si>
-    <t>Coletor não responde, Coletor não se move, Coletor não funciona corretamente</t>
-  </si>
-  <si>
-    <t>Alarme de som, Alerta de barulho, Alerta de falta de sinal, Alerta sonoro</t>
-  </si>
-  <si>
-    <t>Alerta de carga mínima, Alerta de carga insuficiente, Alerta de pouca carga</t>
-  </si>
-  <si>
-    <t>Teclado não funciona, Teclas não respondem, Teclado não responde corretamente</t>
-  </si>
-  <si>
-    <t>Problema de conexão Wi-Fi, Falha na conexão Wi-Fi, Wi-Fi não funciona</t>
-  </si>
-  <si>
-    <t>Problema de conexão USB, Falha na conexão USB, USB não funciona</t>
-  </si>
-  <si>
-    <t>Dados não são salvos, Medições não são salvas, Problema de armazenamento</t>
-  </si>
-  <si>
-    <t>Equipamento não funciona, Equipamento não inicializa, Equipamento não acende</t>
-  </si>
-  <si>
-    <t>Imagem embaçada, Imagem não nítida, Imagem não focada</t>
-  </si>
-  <si>
-    <t>Imagem termográfica em preto, Termograma sem imagem, Termograma sem leitura</t>
-  </si>
-  <si>
-    <t>Termograma não é salvo, Problema de armazenamento de termograma, Dados termográficos não são armazenados</t>
-  </si>
-  <si>
-    <t>Bateria não carrega, Problema de carregamento, Problema na fonte de energia</t>
-  </si>
-  <si>
-    <t>Problema com a câmera, Câmera não responde, Câmera não grava corretamente</t>
-  </si>
-  <si>
-    <t>Imagem da câmera desfocada, Vídeos da câmera sem qualidade, Vídeos da câmera não nítidos</t>
-  </si>
-  <si>
-    <t>Problema de conexão USB da câmera, Falha na conexão USB da câmera, Câmera não se comunica com o computador</t>
-  </si>
-  <si>
-    <t>Bateria da câmera não dura, Problema de bateria da câmera, Câmera não segura carga</t>
-  </si>
-  <si>
-    <t>Pouca carga na bateria, Bateria descarregando, Bateria fraca</t>
-  </si>
-  <si>
-    <t>Problema de leitura de corrente, Falha na leitura de corrente, Corrente não é lida</t>
-  </si>
-  <si>
-    <t>Falha de conexão</t>
-  </si>
-  <si>
-    <t>Conexão lenta / Instável / Problemas de rede</t>
-  </si>
-  <si>
-    <t>Falha de comunicação</t>
-  </si>
-  <si>
-    <t>Problemas com integração do RDP</t>
-  </si>
-  <si>
-    <t>Falha na integração do RDP com o sistema Mysemeq</t>
-  </si>
-  <si>
-    <t>Falha na geração de ordem de serviço na aplicação</t>
-  </si>
-  <si>
-    <t>Erro de gateway</t>
-  </si>
-  <si>
-    <t>Tempo limite de requisição excedido</t>
-  </si>
-  <si>
-    <t>API fora do ar / indisponível</t>
-  </si>
-  <si>
-    <t>Problemas com endpoints específicos da API</t>
-  </si>
-  <si>
-    <t>Problemas com retorno de dados na API</t>
-  </si>
-  <si>
-    <t>Lentidão no sistema / Baixo desempenho</t>
-  </si>
-  <si>
-    <t>Falha ao carregar a página</t>
-  </si>
-  <si>
-    <t>Falha ao carregar gráfico de pizza</t>
-  </si>
-  <si>
-    <t>Falha ao carregar priorização</t>
-  </si>
-  <si>
-    <t>Interface do sistema inacessível</t>
-  </si>
-  <si>
-    <t>Sistema apresentando lentidão</t>
-  </si>
-  <si>
-    <t>Problemas ao fazer login no aplicativo</t>
-  </si>
-  <si>
-    <t>Problemas com login</t>
-  </si>
-  <si>
-    <t>Problemas com acesso do usuário</t>
-  </si>
-  <si>
-    <t>Dados apresentando informações desatualizadas</t>
-  </si>
-  <si>
-    <t>Portal do sistema apresentando lentidão</t>
-  </si>
-  <si>
-    <t>Falha ao carregar o portal do sistema</t>
-  </si>
-  <si>
-    <t>Falha ao carregar a árvore do sistema</t>
-  </si>
-  <si>
-    <t>Problemas com medidas de tendência do analisador / desalinhadas</t>
-  </si>
-  <si>
-    <t>servidor indisponível, erro 502, gateway ruim, tempo limite excedido</t>
-  </si>
-  <si>
-    <t>tempo limite de solicitação, servidor não responde, tempo limite esgotado</t>
-  </si>
-  <si>
-    <t>api fora do ar, api não está funcionando, api inacessível</t>
-  </si>
-  <si>
-    <t>api endpoint fora do ar, endpoint indisponível, endpoint inacessível</t>
-  </si>
-  <si>
-    <t>api sem resposta, api não responde, sem retorno da api, sem mensagem de erro</t>
-  </si>
-  <si>
-    <t>lentidão na rede, conexão lenta, baixa velocidade de rede</t>
-  </si>
-  <si>
-    <t>site não carrega, página inacessível, erro ao carregar a página</t>
-  </si>
-  <si>
-    <t>gráfico não aparece, gráfico não carrega, erro no gráfico</t>
-  </si>
-  <si>
-    <t>lista de priorização não aparece, erro na lista de priorização</t>
-  </si>
-  <si>
-    <t>sensor sem comunicação bidirecional, sem comunicação de ida e volta</t>
-  </si>
-  <si>
-    <t>gateway não acessível, gateway inacessível, gateway sem comunicação</t>
-  </si>
-  <si>
-    <t>sem conexão com a internet, internet do cliente inacessível, internet do cliente sem comunicação</t>
-  </si>
-  <si>
-    <t>conexão perdida, conexão interrompida, desconectado da rede</t>
-  </si>
-  <si>
-    <t>sensor sem comunicação, sem comunicação com o sensor, sensor offline</t>
-  </si>
-  <si>
-    <t>data e hora do gateway incorretas, gateway com data e hora erradas</t>
-  </si>
-  <si>
-    <t>gateway conectado mas não aparece na interface, sem comunicação do gateway na interface</t>
-  </si>
-  <si>
     <t>coleta periodica offline</t>
   </si>
   <si>
-    <t>Alerta de sobrecarga, Alerta de carga máxima, Alerta de excesso de carga,coletor está com alerta de sobrecarga,coletor está com alerta de overload</t>
-  </si>
-  <si>
-    <t>Falha ao carregar priorização, priorização do mysemeq não carrega</t>
+    <t>coletor, funciona, inicializa, acende, liga</t>
+  </si>
+  <si>
+    <t>Alerta, ruído, ausência, sinal, interrupção, barulho, falha</t>
+  </si>
+  <si>
+    <t>Alerta, overload, sobrecarga, excesso, carga, peso, limite</t>
+  </si>
+  <si>
+    <t>http, 408, timeout</t>
+  </si>
+  <si>
+    <t>api, indisponível</t>
+  </si>
+  <si>
+    <t>não gerou ordem de serviço na aplicação</t>
+  </si>
+  <si>
+    <t>sistema, lento, demora, travamento</t>
+  </si>
+  <si>
+    <t>login, app, falha, erro</t>
+  </si>
+  <si>
+    <t>login, falha, erro</t>
+  </si>
+  <si>
+    <t>erro, dados, desatualizados</t>
+  </si>
+  <si>
+    <t>lentidão, portal, carregando</t>
+  </si>
+  <si>
+    <t>erro, portal, carregamento</t>
+  </si>
+  <si>
+    <t>erro, árvore, carregamento</t>
+  </si>
+  <si>
+    <t>erro, tendência, análise</t>
+  </si>
+  <si>
+    <t>erro, login, acesso, usuário, acesso</t>
+  </si>
+  <si>
+    <t>api, endpoint, inacessível</t>
+  </si>
+  <si>
+    <t>Internet, conexão, cliente</t>
+  </si>
+  <si>
+    <t>Comunicação, sensor</t>
+  </si>
+  <si>
+    <t>GW, gateway, online, data, hora</t>
+  </si>
+  <si>
+    <t>Gateway, interface, conexão</t>
+  </si>
+  <si>
+    <t>GW, gateway, interface, conexão</t>
+  </si>
+  <si>
+    <t>Coletor, travado, emperrado, funciona, liga</t>
+  </si>
+  <si>
+    <t>Alerta, underload, carga, baixa, reduzida, menor</t>
+  </si>
+  <si>
+    <t>Falha, teclado, membrana, funciona, responde</t>
+  </si>
+  <si>
+    <t>Problema, conexão, internet, wifi, fio, rede, wireless</t>
+  </si>
+  <si>
+    <t>Problema, conexão, internet, usb, cabo, fio, conectividade</t>
+  </si>
+  <si>
+    <t>salva, medições, medidas, dados, gravação, registro, armazenamento</t>
+  </si>
+  <si>
+    <t>Equipamento, funciona, inicializa, acende</t>
+  </si>
+  <si>
+    <t>Imagem, embaçada, nítida, focada, nítidez</t>
+  </si>
+  <si>
+    <t>Imagem, termográfica, termograma, preto, leitura, apagado, vídeo, escuro, escura</t>
+  </si>
+  <si>
+    <t>Termograma, salvo, armazenamento, Dados, termográficos, armazenados, salva</t>
+  </si>
+  <si>
+    <t>Bateria, carrega, carregamento, fonte, energia</t>
+  </si>
+  <si>
+    <t>câmera, responde, grava, corretamente, funciona, termográfica, pega, pegar, parou</t>
+  </si>
+  <si>
+    <t>Imagem, câmera, desfocada, Vídeos, qualidade, nítidos, em baçada, embaçado, lavados, lavado</t>
+  </si>
+  <si>
+    <t>conexão, USB, câmera, Falha, conexão, comunica, computador, conecta, conectar</t>
+  </si>
+  <si>
+    <t>Bateria, câmera, dura,  segura, carga</t>
+  </si>
+  <si>
+    <t>Equipamento, funciona, inicializa, acende, liga</t>
+  </si>
+  <si>
+    <t>Imagem, embaçada, nítida, focada, foco, lavado</t>
+  </si>
+  <si>
+    <t>Imagem, termográfica, preto, Termograma, imagem, leitura, apagado, escuro</t>
+  </si>
+  <si>
+    <t>Termograma, salvo, armazenamento, Dados, termográficos, armazenados</t>
+  </si>
+  <si>
+    <t>câmera, responde, grava, corretamente</t>
+  </si>
+  <si>
+    <t>imagem, câmera, desfocada,desfoco, Vídeos, qualidade, nítidos, lavado</t>
+  </si>
+  <si>
+    <t>conexão, USB, câmera, comunica, computador, conecta</t>
+  </si>
+  <si>
+    <t>Bateria, câmera, dura, segura, carga</t>
+  </si>
+  <si>
+    <t>Pouca, carga, bateria, descarregando, fraca, descarrega</t>
+  </si>
+  <si>
+    <t>leitura, corrente, Falha, lida, lê, conversa</t>
+  </si>
+  <si>
+    <t>120, link, down, conexão, interrompida, rede</t>
+  </si>
+  <si>
+    <t>120, perda, pacote, lentidão, velocidade, baixa, conexão, lenta</t>
+  </si>
+  <si>
+    <t>comunicação, conexão, sinal, resposta</t>
+  </si>
+  <si>
+    <t>rdp, integração, erro, integrado</t>
+  </si>
+  <si>
+    <t>rdp, baixa, mysemeq, integração, erro, integrada</t>
+  </si>
+  <si>
+    <t>ordem, serviço, aplicação, gerou, erro</t>
+  </si>
+  <si>
+    <t>http, 502, bad, gateway, erro, rede</t>
+  </si>
+  <si>
+    <t>http, 408, timeout, erro, rede</t>
+  </si>
+  <si>
+    <t>api, indisponível, erro, rede</t>
+  </si>
+  <si>
+    <t>api, endpoint, inacessível, erro, rede</t>
+  </si>
+  <si>
+    <t>api, resposta, erro</t>
+  </si>
+  <si>
+    <t>lentidão, demora, travamento, lento</t>
+  </si>
+  <si>
+    <t>página, carrega, erro</t>
+  </si>
+  <si>
+    <t>gráfico, pizza, carrega, erro</t>
+  </si>
+  <si>
+    <t>priorização, carrega, erro</t>
+  </si>
+  <si>
+    <t>interface, inacessível, erro, rede</t>
+  </si>
+  <si>
+    <t>http, 502, bad, gateway</t>
+  </si>
+  <si>
+    <t>api, endpoint, acessível</t>
+  </si>
+  <si>
+    <t>api, retorna, dados, mensagem</t>
+  </si>
+  <si>
+    <t>lentidão, lento, travando</t>
+  </si>
+  <si>
+    <t>página, carrega</t>
+  </si>
+  <si>
+    <t>gráfico, pizza, carrega</t>
+  </si>
+  <si>
+    <t>priorização, carrega</t>
+  </si>
+  <si>
+    <t>api, resposta</t>
+  </si>
+  <si>
+    <t>lentidão, baixo, desempenho</t>
+  </si>
+  <si>
+    <t>sensor, vínculo, aplicado</t>
+  </si>
+  <si>
+    <t>gateway, interface, entra</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -592,12 +625,6 @@
       <name val="MS Shell Dlg 2"/>
     </font>
     <font>
-      <sz val="12"/>
-      <name val="Segoe UI"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
       <sz val="12"/>
       <name val="Segoe UI"/>
       <family val="2"/>
@@ -709,7 +736,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -723,13 +750,10 @@
     <xf numFmtId="0" fontId="4" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1046,8 +1070,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E221B1-E974-48EE-8D2F-4D47A5EBE7F7}">
   <dimension ref="A1:K168"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H5" sqref="H5"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="J167" sqref="J167"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1064,7 +1088,7 @@
     <col min="14" max="14" width="38.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>7</v>
       </c>
@@ -1087,9 +1111,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>8</v>
@@ -1104,17 +1128,15 @@
         <v>11</v>
       </c>
       <c r="F2" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="36" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>115</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="J2" s="3"/>
-      <c r="K2" s="4"/>
-    </row>
-    <row r="3" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
-        <v>175</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>8</v>
@@ -1129,17 +1151,15 @@
         <v>12</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>116</v>
+        <v>137</v>
       </c>
       <c r="G3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J3" s="3"/>
-      <c r="K3" s="4"/>
-    </row>
-    <row r="4" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:9" ht="54" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>8</v>
@@ -1159,12 +1179,10 @@
       <c r="G4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J4" s="3"/>
-      <c r="K4" s="4"/>
-    </row>
-    <row r="5" spans="1:11" ht="126.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:9" ht="54" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>8</v>
@@ -1179,18 +1197,16 @@
         <v>14</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="G5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="I5" s="7"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="4"/>
-    </row>
-    <row r="6" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I5" s="6"/>
+    </row>
+    <row r="6" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>8</v>
@@ -1205,17 +1221,15 @@
         <v>15</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>118</v>
+        <v>138</v>
       </c>
       <c r="G6" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J6" s="3"/>
-      <c r="K6" s="4"/>
-    </row>
-    <row r="7" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:9" ht="36" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>8</v>
@@ -1230,17 +1244,15 @@
         <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>119</v>
+        <v>139</v>
       </c>
       <c r="G7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J7" s="5"/>
-      <c r="K7" s="4"/>
-    </row>
-    <row r="8" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:9" ht="54" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -1255,17 +1267,15 @@
         <v>17</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>120</v>
+        <v>140</v>
       </c>
       <c r="G8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J8" s="3"/>
-      <c r="K8" s="4"/>
-    </row>
-    <row r="9" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:9" ht="54" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>8</v>
@@ -1280,17 +1290,15 @@
         <v>18</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>121</v>
+        <v>141</v>
       </c>
       <c r="G9" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="3"/>
-      <c r="K9" s="4"/>
-    </row>
-    <row r="10" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:9" ht="54" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>8</v>
@@ -1305,17 +1313,15 @@
         <v>19</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>122</v>
+        <v>142</v>
       </c>
       <c r="G10" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J10" s="3"/>
-      <c r="K10" s="4"/>
-    </row>
-    <row r="11" spans="1:11" ht="33.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:9" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>8</v>
@@ -1330,17 +1336,15 @@
         <v>22</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>123</v>
+        <v>143</v>
       </c>
       <c r="G11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="4"/>
-    </row>
-    <row r="12" spans="1:11" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:9" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>8</v>
@@ -1355,17 +1359,15 @@
         <v>23</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>124</v>
+        <v>144</v>
       </c>
       <c r="G12" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="4"/>
-    </row>
-    <row r="13" spans="1:11" ht="29.25" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>8</v>
@@ -1380,17 +1382,15 @@
         <v>24</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>125</v>
+        <v>145</v>
       </c>
       <c r="G13" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J13" s="3"/>
-      <c r="K13" s="4"/>
-    </row>
-    <row r="14" spans="1:11" ht="108.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>8</v>
@@ -1405,17 +1405,15 @@
         <v>25</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>126</v>
+        <v>146</v>
       </c>
       <c r="G14" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J14" s="3"/>
-      <c r="K14" s="4"/>
-    </row>
-    <row r="15" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:9" ht="54" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>8</v>
@@ -1430,17 +1428,15 @@
         <v>26</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="3"/>
-      <c r="K15" s="4"/>
-    </row>
-    <row r="16" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:9" ht="72" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>8</v>
@@ -1455,17 +1451,15 @@
         <v>27</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>128</v>
+        <v>148</v>
       </c>
       <c r="G16" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J16" s="3"/>
-      <c r="K16" s="4"/>
-    </row>
-    <row r="17" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="17" spans="1:7" ht="90" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>8</v>
@@ -1480,17 +1474,15 @@
         <v>28</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>129</v>
+        <v>149</v>
       </c>
       <c r="G17" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J17" s="3"/>
-      <c r="K17" s="4"/>
-    </row>
-    <row r="18" spans="1:11" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="18" spans="1:7" ht="72" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>8</v>
@@ -1505,17 +1497,15 @@
         <v>29</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>130</v>
+        <v>150</v>
       </c>
       <c r="G18" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J18" s="3"/>
-      <c r="K18" s="4"/>
-    </row>
-    <row r="19" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="19" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>8</v>
@@ -1530,17 +1520,15 @@
         <v>30</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>131</v>
+        <v>151</v>
       </c>
       <c r="G19" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J19" s="3"/>
-      <c r="K19" s="4"/>
-    </row>
-    <row r="20" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="20" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>8</v>
@@ -1555,17 +1543,15 @@
         <v>22</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>123</v>
+        <v>152</v>
       </c>
       <c r="G20" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J20" s="3"/>
-      <c r="K20" s="4"/>
-    </row>
-    <row r="21" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="21" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>8</v>
@@ -1580,17 +1566,15 @@
         <v>23</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>124</v>
+        <v>153</v>
       </c>
       <c r="G21" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J21" s="3"/>
-      <c r="K21" s="4"/>
-    </row>
-    <row r="22" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    </row>
+    <row r="22" spans="1:7" ht="72" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>8</v>
@@ -1605,15 +1589,15 @@
         <v>24</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>125</v>
+        <v>154</v>
       </c>
       <c r="G22" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="108" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" ht="72" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>8</v>
@@ -1628,15 +1612,15 @@
         <v>25</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>126</v>
+        <v>155</v>
       </c>
       <c r="G23" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" ht="54" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>8</v>
@@ -1651,15 +1635,15 @@
         <v>26</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>127</v>
+        <v>147</v>
       </c>
       <c r="G24" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>8</v>
@@ -1674,15 +1658,15 @@
         <v>27</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>128</v>
+        <v>156</v>
       </c>
       <c r="G25" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" ht="54" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>8</v>
@@ -1697,15 +1681,15 @@
         <v>28</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>129</v>
+        <v>157</v>
       </c>
       <c r="G26" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="90" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" ht="54" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>8</v>
@@ -1720,15 +1704,15 @@
         <v>29</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="G27" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>8</v>
@@ -1743,15 +1727,15 @@
         <v>30</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="G28" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="54" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" ht="54" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>8</v>
@@ -1759,22 +1743,22 @@
       <c r="C29" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>33</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>34</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="G29" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="72" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
-        <v>175</v>
+        <v>115</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>8</v>
@@ -1789,13 +1773,13 @@
         <v>35</v>
       </c>
       <c r="F30" s="2" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="G30" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>113</v>
       </c>
@@ -1812,15 +1796,13 @@
         <v>39</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="G31" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J31" s="3"/>
-      <c r="K31" s="4"/>
-    </row>
-    <row r="32" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="32" spans="1:7" ht="54" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>113</v>
       </c>
@@ -1837,15 +1819,13 @@
         <v>40</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="G32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="J32" s="3"/>
-      <c r="K32" s="4"/>
-    </row>
-    <row r="33" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
         <v>113</v>
       </c>
@@ -1862,7 +1842,7 @@
         <v>39</v>
       </c>
       <c r="F33" s="2" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="G33" s="2" t="s">
         <v>4</v>
@@ -1870,7 +1850,7 @@
       <c r="J33" s="3"/>
       <c r="K33" s="4"/>
     </row>
-    <row r="34" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
         <v>113</v>
       </c>
@@ -1887,7 +1867,7 @@
         <v>40</v>
       </c>
       <c r="F34" s="2" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="G34" s="2" t="s">
         <v>4</v>
@@ -1895,7 +1875,7 @@
       <c r="J34" s="3"/>
       <c r="K34" s="4"/>
     </row>
-    <row r="35" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
         <v>113</v>
       </c>
@@ -1912,7 +1892,7 @@
         <v>39</v>
       </c>
       <c r="F35" s="2" t="s">
-        <v>134</v>
+        <v>162</v>
       </c>
       <c r="G35" s="2" t="s">
         <v>4</v>
@@ -1920,7 +1900,7 @@
       <c r="J35" s="3"/>
       <c r="K35" s="4"/>
     </row>
-    <row r="36" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
         <v>113</v>
       </c>
@@ -1937,7 +1917,7 @@
         <v>40</v>
       </c>
       <c r="F36" s="2" t="s">
-        <v>135</v>
+        <v>163</v>
       </c>
       <c r="G36" s="2" t="s">
         <v>4</v>
@@ -1945,7 +1925,7 @@
       <c r="J36" s="3"/>
       <c r="K36" s="4"/>
     </row>
-    <row r="37" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
         <v>113</v>
       </c>
@@ -1962,7 +1942,7 @@
         <v>48</v>
       </c>
       <c r="F37" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="G37" s="2" t="s">
         <v>4</v>
@@ -1970,7 +1950,7 @@
       <c r="J37" s="3"/>
       <c r="K37" s="4"/>
     </row>
-    <row r="38" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
         <v>113</v>
       </c>
@@ -1987,7 +1967,7 @@
         <v>48</v>
       </c>
       <c r="F38" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="G38" s="2" t="s">
         <v>4</v>
@@ -1995,7 +1975,7 @@
       <c r="J38" s="3"/>
       <c r="K38" s="4"/>
     </row>
-    <row r="39" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
         <v>113</v>
       </c>
@@ -2012,7 +1992,7 @@
         <v>48</v>
       </c>
       <c r="F39" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="G39" s="2" t="s">
         <v>4</v>
@@ -2020,7 +2000,7 @@
       <c r="J39" s="3"/>
       <c r="K39" s="4"/>
     </row>
-    <row r="40" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
         <v>113</v>
       </c>
@@ -2037,7 +2017,7 @@
         <v>48</v>
       </c>
       <c r="F40" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="G40" s="2" t="s">
         <v>4</v>
@@ -2045,7 +2025,7 @@
       <c r="J40" s="3"/>
       <c r="K40" s="4"/>
     </row>
-    <row r="41" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
         <v>113</v>
       </c>
@@ -2062,7 +2042,7 @@
         <v>48</v>
       </c>
       <c r="F41" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="G41" s="2" t="s">
         <v>4</v>
@@ -2070,7 +2050,7 @@
       <c r="J41" s="3"/>
       <c r="K41" s="4"/>
     </row>
-    <row r="42" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
         <v>113</v>
       </c>
@@ -2087,7 +2067,7 @@
         <v>48</v>
       </c>
       <c r="F42" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="G42" s="2" t="s">
         <v>4</v>
@@ -2095,7 +2075,7 @@
       <c r="J42" s="3"/>
       <c r="K42" s="4"/>
     </row>
-    <row r="43" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="2" t="s">
         <v>113</v>
       </c>
@@ -2112,7 +2092,7 @@
         <v>48</v>
       </c>
       <c r="F43" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="G43" s="2" t="s">
         <v>4</v>
@@ -2120,7 +2100,7 @@
       <c r="J43" s="3"/>
       <c r="K43" s="4"/>
     </row>
-    <row r="44" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="2" t="s">
         <v>113</v>
       </c>
@@ -2137,7 +2117,7 @@
         <v>48</v>
       </c>
       <c r="F44" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="G44" s="2" t="s">
         <v>4</v>
@@ -2145,7 +2125,7 @@
       <c r="J44" s="3"/>
       <c r="K44" s="4"/>
     </row>
-    <row r="45" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="2" t="s">
         <v>113</v>
       </c>
@@ -2162,7 +2142,7 @@
         <v>48</v>
       </c>
       <c r="F45" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="G45" s="2" t="s">
         <v>4</v>
@@ -2170,7 +2150,7 @@
       <c r="J45" s="3"/>
       <c r="K45" s="4"/>
     </row>
-    <row r="46" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="2" t="s">
         <v>113</v>
       </c>
@@ -2187,7 +2167,7 @@
         <v>48</v>
       </c>
       <c r="F46" s="2" t="s">
-        <v>136</v>
+        <v>164</v>
       </c>
       <c r="G46" s="2" t="s">
         <v>4</v>
@@ -2212,7 +2192,7 @@
         <v>58</v>
       </c>
       <c r="F47" s="2" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="G47" s="2" t="s">
         <v>4</v>
@@ -2220,7 +2200,7 @@
       <c r="J47" s="3"/>
       <c r="K47" s="4"/>
     </row>
-    <row r="48" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="2" t="s">
         <v>54</v>
       </c>
@@ -2237,7 +2217,7 @@
         <v>60</v>
       </c>
       <c r="F48" s="2" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="G48" s="2" t="s">
         <v>4</v>
@@ -2245,7 +2225,7 @@
       <c r="J48" s="3"/>
       <c r="K48" s="4"/>
     </row>
-    <row r="49" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="2" t="s">
         <v>54</v>
       </c>
@@ -2259,10 +2239,10 @@
         <v>61</v>
       </c>
       <c r="E49" s="2" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="F49" s="2" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="G49" s="2" t="s">
         <v>4</v>
@@ -2270,7 +2250,7 @@
       <c r="J49" s="3"/>
       <c r="K49" s="4"/>
     </row>
-    <row r="50" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="2" t="s">
         <v>54</v>
       </c>
@@ -2284,10 +2264,10 @@
         <v>63</v>
       </c>
       <c r="E50" s="2" t="s">
-        <v>62</v>
+        <v>121</v>
       </c>
       <c r="F50" s="2" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="G50" s="2" t="s">
         <v>4</v>
@@ -2295,7 +2275,7 @@
       <c r="J50" s="3"/>
       <c r="K50" s="4"/>
     </row>
-    <row r="51" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A51" s="2" t="s">
         <v>54</v>
       </c>
@@ -2312,7 +2292,7 @@
         <v>65</v>
       </c>
       <c r="F51" s="2" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="G51" s="2" t="s">
         <v>4</v>
@@ -2337,7 +2317,7 @@
         <v>66</v>
       </c>
       <c r="F52" s="2" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="G52" s="2" t="s">
         <v>4</v>
@@ -2362,7 +2342,7 @@
         <v>67</v>
       </c>
       <c r="F53" s="2" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="G53" s="2" t="s">
         <v>4</v>
@@ -2387,7 +2367,7 @@
         <v>68</v>
       </c>
       <c r="F54" s="2" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="G54" s="2" t="s">
         <v>4</v>
@@ -2412,7 +2392,7 @@
         <v>69</v>
       </c>
       <c r="F55" s="2" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="G55" s="2" t="s">
         <v>4</v>
@@ -2437,7 +2417,7 @@
         <v>70</v>
       </c>
       <c r="F56" s="2" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="G56" s="2" t="s">
         <v>4</v>
@@ -2460,7 +2440,7 @@
         <v>71</v>
       </c>
       <c r="F57" s="2" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="G57" s="2" t="s">
         <v>4</v>
@@ -2483,13 +2463,13 @@
         <v>72</v>
       </c>
       <c r="F58" s="2" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="G58" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="59" spans="1:11" ht="54" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:11" ht="18" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>54</v>
       </c>
@@ -2506,13 +2486,13 @@
         <v>73</v>
       </c>
       <c r="F59" s="2" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G59" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="60" spans="1:11" ht="18" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:11" ht="36" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>54</v>
       </c>
@@ -2529,7 +2509,7 @@
         <v>65</v>
       </c>
       <c r="F60" s="2" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="G60" s="2" t="s">
         <v>4</v>
@@ -2552,7 +2532,7 @@
         <v>66</v>
       </c>
       <c r="F61" s="2" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="G61" s="2" t="s">
         <v>4</v>
@@ -2575,7 +2555,7 @@
         <v>67</v>
       </c>
       <c r="F62" s="2" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="G62" s="2" t="s">
         <v>4</v>
@@ -2598,7 +2578,7 @@
         <v>68</v>
       </c>
       <c r="F63" s="2" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="G63" s="2" t="s">
         <v>4</v>
@@ -2621,7 +2601,7 @@
         <v>69</v>
       </c>
       <c r="F64" s="2" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="G64" s="2" t="s">
         <v>4</v>
@@ -2644,7 +2624,7 @@
         <v>70</v>
       </c>
       <c r="F65" s="2" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="G65" s="2" t="s">
         <v>4</v>
@@ -2667,7 +2647,7 @@
         <v>71</v>
       </c>
       <c r="F66" s="2" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="G66" s="2" t="s">
         <v>4</v>
@@ -2690,13 +2670,13 @@
         <v>72</v>
       </c>
       <c r="F67" s="2" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="G67" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>54</v>
       </c>
@@ -2713,7 +2693,7 @@
         <v>73</v>
       </c>
       <c r="F68" s="2" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="G68" s="2" t="s">
         <v>4</v>
@@ -2736,7 +2716,7 @@
         <v>76</v>
       </c>
       <c r="F69" s="2" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="G69" s="2" t="s">
         <v>4</v>
@@ -2759,7 +2739,7 @@
         <v>76</v>
       </c>
       <c r="F70" s="2" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="G70" s="2" t="s">
         <v>4</v>
@@ -2782,13 +2762,13 @@
         <v>77</v>
       </c>
       <c r="F71" s="2" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="G71" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="72" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>54</v>
       </c>
@@ -2805,13 +2785,13 @@
         <v>79</v>
       </c>
       <c r="F72" s="2" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G72" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="73" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>54</v>
       </c>
@@ -2828,7 +2808,7 @@
         <v>79</v>
       </c>
       <c r="F73" s="2" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G73" s="2" t="s">
         <v>4</v>
@@ -2851,7 +2831,7 @@
         <v>82</v>
       </c>
       <c r="F74" s="2" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="G74" s="2" t="s">
         <v>4</v>
@@ -2874,13 +2854,13 @@
         <v>83</v>
       </c>
       <c r="F75" s="2" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="G75" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="76" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>54</v>
       </c>
@@ -2897,7 +2877,7 @@
         <v>86</v>
       </c>
       <c r="F76" s="2" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="G76" s="2" t="s">
         <v>4</v>
@@ -2920,7 +2900,7 @@
         <v>83</v>
       </c>
       <c r="F77" s="2" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="G77" s="2" t="s">
         <v>4</v>
@@ -2943,13 +2923,13 @@
         <v>89</v>
       </c>
       <c r="F78" s="2" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="G78" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>54</v>
       </c>
@@ -2966,7 +2946,7 @@
         <v>90</v>
       </c>
       <c r="F79" s="2" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="G79" s="2" t="s">
         <v>4</v>
@@ -2989,7 +2969,7 @@
         <v>91</v>
       </c>
       <c r="F80" s="2" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="G80" s="2" t="s">
         <v>4</v>
@@ -3012,13 +2992,13 @@
         <v>89</v>
       </c>
       <c r="F81" s="2" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="G81" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="82" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>54</v>
       </c>
@@ -3035,7 +3015,7 @@
         <v>90</v>
       </c>
       <c r="F82" s="2" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="G82" s="2" t="s">
         <v>4</v>
@@ -3058,7 +3038,7 @@
         <v>91</v>
       </c>
       <c r="F83" s="2" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="G83" s="2" t="s">
         <v>4</v>
@@ -3081,13 +3061,13 @@
         <v>89</v>
       </c>
       <c r="F84" s="2" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="G84" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="85" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>54</v>
       </c>
@@ -3104,7 +3084,7 @@
         <v>90</v>
       </c>
       <c r="F85" s="2" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="G85" s="2" t="s">
         <v>4</v>
@@ -3127,13 +3107,13 @@
         <v>91</v>
       </c>
       <c r="F86" s="2" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="G86" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="87" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>54</v>
       </c>
@@ -3150,7 +3130,7 @@
         <v>95</v>
       </c>
       <c r="F87" s="2" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="G87" s="2" t="s">
         <v>4</v>
@@ -3173,13 +3153,13 @@
         <v>58</v>
       </c>
       <c r="F88" s="2" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
       <c r="G88" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>94</v>
       </c>
@@ -3196,13 +3176,13 @@
         <v>60</v>
       </c>
       <c r="F89" s="2" t="s">
-        <v>138</v>
+        <v>166</v>
       </c>
       <c r="G89" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>94</v>
       </c>
@@ -3219,13 +3199,13 @@
         <v>62</v>
       </c>
       <c r="F90" s="2" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="G90" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>94</v>
       </c>
@@ -3242,13 +3222,13 @@
         <v>62</v>
       </c>
       <c r="F91" s="2" t="s">
-        <v>139</v>
+        <v>167</v>
       </c>
       <c r="G91" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>94</v>
       </c>
@@ -3265,7 +3245,7 @@
         <v>65</v>
       </c>
       <c r="F92" s="2" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="G92" s="2" t="s">
         <v>4</v>
@@ -3288,7 +3268,7 @@
         <v>66</v>
       </c>
       <c r="F93" s="2" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="G93" s="2" t="s">
         <v>4</v>
@@ -3311,7 +3291,7 @@
         <v>67</v>
       </c>
       <c r="F94" s="2" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="G94" s="2" t="s">
         <v>4</v>
@@ -3334,7 +3314,7 @@
         <v>68</v>
       </c>
       <c r="F95" s="2" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="G95" s="2" t="s">
         <v>4</v>
@@ -3357,7 +3337,7 @@
         <v>69</v>
       </c>
       <c r="F96" s="2" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="G96" s="2" t="s">
         <v>4</v>
@@ -3380,7 +3360,7 @@
         <v>70</v>
       </c>
       <c r="F97" s="2" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="G97" s="2" t="s">
         <v>4</v>
@@ -3403,7 +3383,7 @@
         <v>71</v>
       </c>
       <c r="F98" s="2" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="G98" s="2" t="s">
         <v>4</v>
@@ -3426,13 +3406,13 @@
         <v>72</v>
       </c>
       <c r="F99" s="2" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="G99" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="100" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>94</v>
       </c>
@@ -3449,13 +3429,13 @@
         <v>73</v>
       </c>
       <c r="F100" s="2" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="G100" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="101" spans="1:7" ht="18" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>94</v>
       </c>
@@ -3472,7 +3452,7 @@
         <v>65</v>
       </c>
       <c r="F101" s="2" t="s">
-        <v>140</v>
+        <v>168</v>
       </c>
       <c r="G101" s="2" t="s">
         <v>4</v>
@@ -3495,7 +3475,7 @@
         <v>66</v>
       </c>
       <c r="F102" s="2" t="s">
-        <v>141</v>
+        <v>169</v>
       </c>
       <c r="G102" s="2" t="s">
         <v>4</v>
@@ -3518,7 +3498,7 @@
         <v>67</v>
       </c>
       <c r="F103" s="2" t="s">
-        <v>142</v>
+        <v>170</v>
       </c>
       <c r="G103" s="2" t="s">
         <v>4</v>
@@ -3541,7 +3521,7 @@
         <v>68</v>
       </c>
       <c r="F104" s="2" t="s">
-        <v>143</v>
+        <v>171</v>
       </c>
       <c r="G104" s="2" t="s">
         <v>4</v>
@@ -3564,7 +3544,7 @@
         <v>69</v>
       </c>
       <c r="F105" s="2" t="s">
-        <v>144</v>
+        <v>172</v>
       </c>
       <c r="G105" s="2" t="s">
         <v>4</v>
@@ -3587,7 +3567,7 @@
         <v>70</v>
       </c>
       <c r="F106" s="2" t="s">
-        <v>145</v>
+        <v>173</v>
       </c>
       <c r="G106" s="2" t="s">
         <v>4</v>
@@ -3610,7 +3590,7 @@
         <v>71</v>
       </c>
       <c r="F107" s="2" t="s">
-        <v>146</v>
+        <v>174</v>
       </c>
       <c r="G107" s="2" t="s">
         <v>4</v>
@@ -3633,13 +3613,13 @@
         <v>72</v>
       </c>
       <c r="F108" s="2" t="s">
-        <v>147</v>
+        <v>175</v>
       </c>
       <c r="G108" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="109" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>94</v>
       </c>
@@ -3656,7 +3636,7 @@
         <v>73</v>
       </c>
       <c r="F109" s="2" t="s">
-        <v>148</v>
+        <v>176</v>
       </c>
       <c r="G109" s="2" t="s">
         <v>4</v>
@@ -3679,7 +3659,7 @@
         <v>76</v>
       </c>
       <c r="F110" s="2" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="G110" s="2" t="s">
         <v>4</v>
@@ -3702,7 +3682,7 @@
         <v>76</v>
       </c>
       <c r="F111" s="2" t="s">
-        <v>149</v>
+        <v>177</v>
       </c>
       <c r="G111" s="2" t="s">
         <v>4</v>
@@ -3725,13 +3705,13 @@
         <v>77</v>
       </c>
       <c r="F112" s="2" t="s">
-        <v>150</v>
+        <v>122</v>
       </c>
       <c r="G112" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="113" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>94</v>
       </c>
@@ -3748,13 +3728,13 @@
         <v>79</v>
       </c>
       <c r="F113" s="2" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G113" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="114" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>94</v>
       </c>
@@ -3771,7 +3751,7 @@
         <v>79</v>
       </c>
       <c r="F114" s="2" t="s">
-        <v>151</v>
+        <v>123</v>
       </c>
       <c r="G114" s="2" t="s">
         <v>4</v>
@@ -3794,7 +3774,7 @@
         <v>82</v>
       </c>
       <c r="F115" s="2" t="s">
-        <v>152</v>
+        <v>124</v>
       </c>
       <c r="G115" s="2" t="s">
         <v>4</v>
@@ -3817,13 +3797,13 @@
         <v>83</v>
       </c>
       <c r="F116" s="2" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="G116" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="117" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>94</v>
       </c>
@@ -3840,7 +3820,7 @@
         <v>86</v>
       </c>
       <c r="F117" s="2" t="s">
-        <v>154</v>
+        <v>125</v>
       </c>
       <c r="G117" s="2" t="s">
         <v>4</v>
@@ -3863,7 +3843,7 @@
         <v>83</v>
       </c>
       <c r="F118" s="2" t="s">
-        <v>153</v>
+        <v>130</v>
       </c>
       <c r="G118" s="2" t="s">
         <v>4</v>
@@ -3886,13 +3866,13 @@
         <v>89</v>
       </c>
       <c r="F119" s="2" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="G119" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="120" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>94</v>
       </c>
@@ -3909,7 +3889,7 @@
         <v>90</v>
       </c>
       <c r="F120" s="2" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="G120" s="2" t="s">
         <v>4</v>
@@ -3932,7 +3912,7 @@
         <v>91</v>
       </c>
       <c r="F121" s="2" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="G121" s="2" t="s">
         <v>4</v>
@@ -3955,13 +3935,13 @@
         <v>89</v>
       </c>
       <c r="F122" s="2" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="G122" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="123" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>94</v>
       </c>
@@ -3978,7 +3958,7 @@
         <v>90</v>
       </c>
       <c r="F123" s="2" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="G123" s="2" t="s">
         <v>4</v>
@@ -4001,7 +3981,7 @@
         <v>91</v>
       </c>
       <c r="F124" s="2" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="G124" s="2" t="s">
         <v>4</v>
@@ -4024,13 +4004,13 @@
         <v>89</v>
       </c>
       <c r="F125" s="2" t="s">
-        <v>155</v>
+        <v>126</v>
       </c>
       <c r="G125" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="126" spans="1:7" ht="36" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>94</v>
       </c>
@@ -4047,7 +4027,7 @@
         <v>90</v>
       </c>
       <c r="F126" s="2" t="s">
-        <v>156</v>
+        <v>127</v>
       </c>
       <c r="G126" s="2" t="s">
         <v>4</v>
@@ -4070,13 +4050,13 @@
         <v>91</v>
       </c>
       <c r="F127" s="2" t="s">
-        <v>157</v>
+        <v>128</v>
       </c>
       <c r="G127" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="128" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>94</v>
       </c>
@@ -4093,13 +4073,13 @@
         <v>95</v>
       </c>
       <c r="F128" s="2" t="s">
-        <v>158</v>
+        <v>129</v>
       </c>
       <c r="G128" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="129" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A129" s="2" t="s">
         <v>8</v>
       </c>
@@ -4116,7 +4096,7 @@
         <v>65</v>
       </c>
       <c r="F129" s="2" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="G129" s="2" t="s">
         <v>4</v>
@@ -4124,7 +4104,7 @@
       <c r="J129" s="3"/>
       <c r="K129" s="4"/>
     </row>
-    <row r="130" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A130" s="2" t="s">
         <v>8</v>
       </c>
@@ -4141,7 +4121,7 @@
         <v>66</v>
       </c>
       <c r="F130" s="2" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="G130" s="2" t="s">
         <v>4</v>
@@ -4149,7 +4129,7 @@
       <c r="J130" s="3"/>
       <c r="K130" s="4"/>
     </row>
-    <row r="131" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A131" s="2" t="s">
         <v>8</v>
       </c>
@@ -4166,7 +4146,7 @@
         <v>67</v>
       </c>
       <c r="F131" s="2" t="s">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="G131" s="2" t="s">
         <v>4</v>
@@ -4174,7 +4154,7 @@
       <c r="J131" s="3"/>
       <c r="K131" s="4"/>
     </row>
-    <row r="132" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A132" s="2" t="s">
         <v>8</v>
       </c>
@@ -4191,7 +4171,7 @@
         <v>68</v>
       </c>
       <c r="F132" s="2" t="s">
-        <v>162</v>
+        <v>179</v>
       </c>
       <c r="G132" s="2" t="s">
         <v>4</v>
@@ -4199,7 +4179,7 @@
       <c r="J132" s="3"/>
       <c r="K132" s="4"/>
     </row>
-    <row r="133" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="2" t="s">
         <v>8</v>
       </c>
@@ -4216,7 +4196,7 @@
         <v>69</v>
       </c>
       <c r="F133" s="2" t="s">
-        <v>163</v>
+        <v>180</v>
       </c>
       <c r="G133" s="2" t="s">
         <v>4</v>
@@ -4224,7 +4204,7 @@
       <c r="J133" s="3"/>
       <c r="K133" s="4"/>
     </row>
-    <row r="134" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="2" t="s">
         <v>8</v>
       </c>
@@ -4241,7 +4221,7 @@
         <v>70</v>
       </c>
       <c r="F134" s="2" t="s">
-        <v>164</v>
+        <v>181</v>
       </c>
       <c r="G134" s="2" t="s">
         <v>4</v>
@@ -4249,7 +4229,7 @@
       <c r="J134" s="3"/>
       <c r="K134" s="4"/>
     </row>
-    <row r="135" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="2" t="s">
         <v>8</v>
       </c>
@@ -4266,7 +4246,7 @@
         <v>71</v>
       </c>
       <c r="F135" s="2" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="G135" s="2" t="s">
         <v>4</v>
@@ -4274,7 +4254,7 @@
       <c r="J135" s="3"/>
       <c r="K135" s="4"/>
     </row>
-    <row r="136" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A136" s="2" t="s">
         <v>8</v>
       </c>
@@ -4291,7 +4271,7 @@
         <v>72</v>
       </c>
       <c r="F136" s="2" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="G136" s="2" t="s">
         <v>4</v>
@@ -4299,7 +4279,7 @@
       <c r="J136" s="3"/>
       <c r="K136" s="4"/>
     </row>
-    <row r="137" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="2" t="s">
         <v>8</v>
       </c>
@@ -4316,7 +4296,7 @@
         <v>73</v>
       </c>
       <c r="F137" s="2" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="G137" s="2" t="s">
         <v>4</v>
@@ -4324,7 +4304,7 @@
       <c r="J137" s="3"/>
       <c r="K137" s="4"/>
     </row>
-    <row r="138" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="2" t="s">
         <v>8</v>
       </c>
@@ -4341,7 +4321,7 @@
         <v>65</v>
       </c>
       <c r="F138" s="2" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="G138" s="2" t="s">
         <v>4</v>
@@ -4349,7 +4329,7 @@
       <c r="J138" s="3"/>
       <c r="K138" s="4"/>
     </row>
-    <row r="139" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="2" t="s">
         <v>8</v>
       </c>
@@ -4366,7 +4346,7 @@
         <v>66</v>
       </c>
       <c r="F139" s="2" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="G139" s="2" t="s">
         <v>4</v>
@@ -4374,7 +4354,7 @@
       <c r="J139" s="3"/>
       <c r="K139" s="4"/>
     </row>
-    <row r="140" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A140" s="2" t="s">
         <v>8</v>
       </c>
@@ -4391,7 +4371,7 @@
         <v>67</v>
       </c>
       <c r="F140" s="2" t="s">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="G140" s="2" t="s">
         <v>4</v>
@@ -4399,7 +4379,7 @@
       <c r="J140" s="3"/>
       <c r="K140" s="4"/>
     </row>
-    <row r="141" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="2" t="s">
         <v>8</v>
       </c>
@@ -4416,7 +4396,7 @@
         <v>68</v>
       </c>
       <c r="F141" s="2" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="G141" s="2" t="s">
         <v>4</v>
@@ -4424,7 +4404,7 @@
       <c r="J141" s="3"/>
       <c r="K141" s="4"/>
     </row>
-    <row r="142" spans="1:11" ht="72.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A142" s="2" t="s">
         <v>8</v>
       </c>
@@ -4441,7 +4421,7 @@
         <v>69</v>
       </c>
       <c r="F142" s="2" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="G142" s="2" t="s">
         <v>4</v>
@@ -4449,7 +4429,7 @@
       <c r="J142" s="3"/>
       <c r="K142" s="4"/>
     </row>
-    <row r="143" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:11" ht="36.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A143" s="2" t="s">
         <v>8</v>
       </c>
@@ -4466,7 +4446,7 @@
         <v>70</v>
       </c>
       <c r="F143" s="2" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="G143" s="2" t="s">
         <v>4</v>
@@ -4474,7 +4454,7 @@
       <c r="J143" s="3"/>
       <c r="K143" s="4"/>
     </row>
-    <row r="144" spans="1:11" ht="54.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:11" ht="18.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A144" s="2" t="s">
         <v>8</v>
       </c>
@@ -4491,7 +4471,7 @@
         <v>71</v>
       </c>
       <c r="F144" s="2" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="G144" s="2" t="s">
         <v>4</v>
@@ -4499,7 +4479,7 @@
       <c r="J144" s="3"/>
       <c r="K144" s="4"/>
     </row>
-    <row r="145" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A145" s="2" t="s">
         <v>8</v>
       </c>
@@ -4516,13 +4496,13 @@
         <v>72</v>
       </c>
       <c r="F145" s="2" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="G145" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="146" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A146" s="2" t="s">
         <v>8</v>
       </c>
@@ -4539,13 +4519,13 @@
         <v>73</v>
       </c>
       <c r="F146" s="2" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="G146" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="147" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A147" s="2" t="s">
         <v>8</v>
       </c>
@@ -4562,13 +4542,13 @@
         <v>65</v>
       </c>
       <c r="F147" s="2" t="s">
-        <v>159</v>
+        <v>178</v>
       </c>
       <c r="G147" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="148" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A148" s="2" t="s">
         <v>8</v>
       </c>
@@ -4585,13 +4565,13 @@
         <v>66</v>
       </c>
       <c r="F148" s="2" t="s">
-        <v>160</v>
+        <v>119</v>
       </c>
       <c r="G148" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="149" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A149" s="2" t="s">
         <v>8</v>
       </c>
@@ -4608,13 +4588,13 @@
         <v>67</v>
       </c>
       <c r="F149" s="2" t="s">
-        <v>161</v>
+        <v>120</v>
       </c>
       <c r="G149" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="150" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A150" s="2" t="s">
         <v>8</v>
       </c>
@@ -4631,13 +4611,13 @@
         <v>68</v>
       </c>
       <c r="F150" s="2" t="s">
-        <v>162</v>
+        <v>131</v>
       </c>
       <c r="G150" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="151" spans="1:7" ht="72" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A151" s="2" t="s">
         <v>8</v>
       </c>
@@ -4654,13 +4634,13 @@
         <v>69</v>
       </c>
       <c r="F151" s="2" t="s">
-        <v>163</v>
+        <v>185</v>
       </c>
       <c r="G151" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="152" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A152" s="2" t="s">
         <v>8</v>
       </c>
@@ -4677,13 +4657,13 @@
         <v>70</v>
       </c>
       <c r="F152" s="2" t="s">
-        <v>164</v>
+        <v>186</v>
       </c>
       <c r="G152" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="153" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A153" s="2" t="s">
         <v>8</v>
       </c>
@@ -4700,13 +4680,13 @@
         <v>71</v>
       </c>
       <c r="F153" s="2" t="s">
-        <v>165</v>
+        <v>182</v>
       </c>
       <c r="G153" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="154" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A154" s="2" t="s">
         <v>8</v>
       </c>
@@ -4723,13 +4703,13 @@
         <v>72</v>
       </c>
       <c r="F154" s="2" t="s">
-        <v>166</v>
+        <v>183</v>
       </c>
       <c r="G154" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="155" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A155" s="2" t="s">
         <v>8</v>
       </c>
@@ -4746,13 +4726,13 @@
         <v>73</v>
       </c>
       <c r="F155" s="2" t="s">
-        <v>167</v>
+        <v>184</v>
       </c>
       <c r="G155" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="156" spans="1:7" ht="72" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:7" ht="54" x14ac:dyDescent="0.25">
       <c r="A156" s="2" t="s">
         <v>8</v>
       </c>
@@ -4769,13 +4749,13 @@
         <v>103</v>
       </c>
       <c r="F156" s="2" t="s">
-        <v>168</v>
+        <v>187</v>
       </c>
       <c r="G156" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="157" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A157" s="2" t="s">
         <v>8</v>
       </c>
@@ -4792,13 +4772,13 @@
         <v>106</v>
       </c>
       <c r="F157" s="2" t="s">
-        <v>169</v>
+        <v>188</v>
       </c>
       <c r="G157" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="158" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A158" s="2" t="s">
         <v>8</v>
       </c>
@@ -4815,13 +4795,13 @@
         <v>107</v>
       </c>
       <c r="F158" s="2" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="G158" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="159" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A159" s="2" t="s">
         <v>8</v>
       </c>
@@ -4838,13 +4818,13 @@
         <v>108</v>
       </c>
       <c r="F159" s="2" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="G159" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="160" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A160" s="2" t="s">
         <v>8</v>
       </c>
@@ -4861,13 +4841,13 @@
         <v>109</v>
       </c>
       <c r="F160" s="2" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="G160" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="161" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A161" s="2" t="s">
         <v>8</v>
       </c>
@@ -4884,13 +4864,13 @@
         <v>110</v>
       </c>
       <c r="F161" s="2" t="s">
-        <v>173</v>
+        <v>134</v>
       </c>
       <c r="G161" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="162" spans="1:7" ht="72" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A162" s="2" t="s">
         <v>8</v>
       </c>
@@ -4907,13 +4887,13 @@
         <v>111</v>
       </c>
       <c r="F162" s="2" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="G162" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="163" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A163" s="2" t="s">
         <v>8</v>
       </c>
@@ -4930,13 +4910,13 @@
         <v>106</v>
       </c>
       <c r="F163" s="2" t="s">
-        <v>169</v>
+        <v>136</v>
       </c>
       <c r="G163" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="164" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A164" s="2" t="s">
         <v>8</v>
       </c>
@@ -4953,13 +4933,13 @@
         <v>107</v>
       </c>
       <c r="F164" s="2" t="s">
-        <v>170</v>
+        <v>132</v>
       </c>
       <c r="G164" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="165" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A165" s="2" t="s">
         <v>8</v>
       </c>
@@ -4976,13 +4956,13 @@
         <v>108</v>
       </c>
       <c r="F165" s="2" t="s">
-        <v>171</v>
+        <v>132</v>
       </c>
       <c r="G165" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="166" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:7" ht="18" x14ac:dyDescent="0.25">
       <c r="A166" s="2" t="s">
         <v>8</v>
       </c>
@@ -4999,13 +4979,13 @@
         <v>109</v>
       </c>
       <c r="F166" s="2" t="s">
-        <v>172</v>
+        <v>133</v>
       </c>
       <c r="G166" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="167" spans="1:7" ht="54" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A167" s="2" t="s">
         <v>8</v>
       </c>
@@ -5022,13 +5002,13 @@
         <v>110</v>
       </c>
       <c r="F167" s="2" t="s">
-        <v>173</v>
+        <v>134</v>
       </c>
       <c r="G167" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="168" spans="1:7" ht="72" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:7" ht="36" x14ac:dyDescent="0.25">
       <c r="A168" s="2" t="s">
         <v>8</v>
       </c>
@@ -5045,7 +5025,7 @@
         <v>111</v>
       </c>
       <c r="F168" s="2" t="s">
-        <v>174</v>
+        <v>135</v>
       </c>
       <c r="G168" s="2" t="s">
         <v>4</v>

</xml_diff>

<commit_message>
criando o modelo corretor ortografico
</commit_message>
<xml_diff>
--- a/database/troubleshooting.xlsx
+++ b/database/troubleshooting.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Semeq\Desktop\ChatbotSemeq\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65C011F1-15E7-4C7B-93D5-E51B89B349CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B24D70F-203F-406B-AB97-444299DF20F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20610" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{9B6CABAE-889F-4735-BD9B-BA414D462F42}"/>
   </bookViews>
@@ -2579,7 +2579,7 @@
   <dimension ref="A1:L192"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="H4" sqref="H4"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>